<commit_message>
Changed dt.time to seconds. Output file in endtime.xlsx
</commit_message>
<xml_diff>
--- a/Screenshots/pilot_ep_1.xlsx
+++ b/Screenshots/pilot_ep_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\linux\scratches\Netflix_image_subtitle_crawler\Screenshots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E4C3DB-B915-431F-A3F2-5BB496CBCABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF15D8B5-8632-4188-906A-4507F24833DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$516</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$517</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -2716,13 +2716,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C516"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="66.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2740,7 +2740,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2481</v>
+        <v>2.4809999999999999</v>
       </c>
       <c r="B2" t="s">
         <v>179</v>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>4780</v>
+        <v>4.78</v>
       </c>
       <c r="B3" t="s">
         <v>275</v>
@@ -2762,7 +2762,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>7087</v>
+        <v>7.0869999999999997</v>
       </c>
       <c r="B4" t="s">
         <v>419</v>
@@ -2770,7 +2770,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>9387</v>
+        <v>9.3870000000000005</v>
       </c>
       <c r="B5" t="s">
         <v>516</v>
@@ -2781,7 +2781,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>11964</v>
+        <v>11.964</v>
       </c>
       <c r="B6" t="s">
         <v>93</v>
@@ -2792,7 +2792,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>14270</v>
+        <v>14.27</v>
       </c>
       <c r="B7" t="s">
         <v>107</v>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>16547</v>
+        <v>16.547000000000001</v>
       </c>
       <c r="B8" t="s">
         <v>117</v>
@@ -2814,7 +2814,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>18882</v>
+        <v>18.882000000000001</v>
       </c>
       <c r="B9" t="s">
         <v>126</v>
@@ -2822,7 +2822,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>21192</v>
+        <v>21.192</v>
       </c>
       <c r="B10" t="s">
         <v>140</v>
@@ -2830,7 +2830,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>23508</v>
+        <v>23.507999999999999</v>
       </c>
       <c r="B11" t="s">
         <v>150</v>
@@ -2838,7 +2838,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>25803</v>
+        <v>25.803000000000001</v>
       </c>
       <c r="B12" t="s">
         <v>160</v>
@@ -2846,7 +2846,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>28103</v>
+        <v>28.103000000000002</v>
       </c>
       <c r="B13" t="s">
         <v>174</v>
@@ -2857,7 +2857,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>30577</v>
+        <v>30.577000000000002</v>
       </c>
       <c r="B14" t="s">
         <v>184</v>
@@ -2868,7 +2868,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>32732</v>
+        <v>32.731999999999999</v>
       </c>
       <c r="B15" t="s">
         <v>194</v>
@@ -2879,7 +2879,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>35052</v>
+        <v>35.052</v>
       </c>
       <c r="B16" t="s">
         <v>208</v>
@@ -2887,7 +2887,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>37352</v>
+        <v>37.351999999999997</v>
       </c>
       <c r="B17" t="s">
         <v>217</v>
@@ -2895,7 +2895,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>39670</v>
+        <v>39.67</v>
       </c>
       <c r="B18" t="s">
         <v>227</v>
@@ -2903,7 +2903,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>41992</v>
+        <v>41.991999999999997</v>
       </c>
       <c r="B19" t="s">
         <v>237</v>
@@ -2911,7 +2911,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>44312</v>
+        <v>44.311999999999998</v>
       </c>
       <c r="B20" t="s">
         <v>250</v>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>46642</v>
+        <v>46.642000000000003</v>
       </c>
       <c r="B21" t="s">
         <v>260</v>
@@ -2930,7 +2930,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>48972</v>
+        <v>48.972000000000001</v>
       </c>
       <c r="B22" t="s">
         <v>270</v>
@@ -2938,7 +2938,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>51285</v>
+        <v>51.284999999999997</v>
       </c>
       <c r="B23" t="s">
         <v>285</v>
@@ -2946,7 +2946,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>53596</v>
+        <v>53.595999999999997</v>
       </c>
       <c r="B24" t="s">
         <v>294</v>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>55907</v>
+        <v>55.906999999999996</v>
       </c>
       <c r="B25" t="s">
         <v>304</v>
@@ -2962,7 +2962,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>58219</v>
+        <v>58.219000000000001</v>
       </c>
       <c r="B26" t="s">
         <v>318</v>
@@ -2973,7 +2973,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>60518</v>
+        <v>60.518000000000001</v>
       </c>
       <c r="B27" t="s">
         <v>327</v>
@@ -2981,7 +2981,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>62829</v>
+        <v>62.829000000000001</v>
       </c>
       <c r="B28" t="s">
         <v>337</v>
@@ -2989,7 +2989,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>65133</v>
+        <v>65.132999999999996</v>
       </c>
       <c r="B29" t="s">
         <v>351</v>
@@ -2997,7 +2997,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>67452</v>
+        <v>67.451999999999998</v>
       </c>
       <c r="B30" t="s">
         <v>361</v>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>69761</v>
+        <v>69.760999999999996</v>
       </c>
       <c r="B31" t="s">
         <v>370</v>
@@ -3013,7 +3013,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>72050</v>
+        <v>72.05</v>
       </c>
       <c r="B32" t="s">
         <v>384</v>
@@ -3024,7 +3024,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>74382</v>
+        <v>74.382000000000005</v>
       </c>
       <c r="B33" t="s">
         <v>394</v>
@@ -3035,7 +3035,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>76682</v>
+        <v>76.682000000000002</v>
       </c>
       <c r="B34" t="s">
         <v>404</v>
@@ -3046,7 +3046,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>78983</v>
+        <v>78.983000000000004</v>
       </c>
       <c r="B35" t="s">
         <v>413</v>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>81293</v>
+        <v>81.293000000000006</v>
       </c>
       <c r="B36" t="s">
         <v>428</v>
@@ -3068,7 +3068,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>83592</v>
+        <v>83.591999999999999</v>
       </c>
       <c r="B37" t="s">
         <v>438</v>
@@ -3079,7 +3079,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>85892</v>
+        <v>85.891999999999996</v>
       </c>
       <c r="B38" t="s">
         <v>448</v>
@@ -3090,7 +3090,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>88212</v>
+        <v>88.212000000000003</v>
       </c>
       <c r="B39" t="s">
         <v>462</v>
@@ -3098,7 +3098,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>90520</v>
+        <v>90.52</v>
       </c>
       <c r="B40" t="s">
         <v>472</v>
@@ -3106,7 +3106,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>92833</v>
+        <v>92.832999999999998</v>
       </c>
       <c r="B41" t="s">
         <v>481</v>
@@ -3117,7 +3117,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>95179</v>
+        <v>95.179000000000002</v>
       </c>
       <c r="B42" t="s">
         <v>496</v>
@@ -3125,7 +3125,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>97508</v>
+        <v>97.507999999999996</v>
       </c>
       <c r="B43" t="s">
         <v>505</v>
@@ -3136,7 +3136,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>99842</v>
+        <v>99.841999999999999</v>
       </c>
       <c r="B44" t="s">
         <v>515</v>
@@ -3147,7 +3147,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>102162</v>
+        <v>102.16200000000001</v>
       </c>
       <c r="B45" t="s">
         <v>15</v>
@@ -3155,7 +3155,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>104495</v>
+        <v>104.495</v>
       </c>
       <c r="B46" t="s">
         <v>25</v>
@@ -3163,7 +3163,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>106812</v>
+        <v>106.812</v>
       </c>
       <c r="B47" t="s">
         <v>35</v>
@@ -3171,7 +3171,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>109128</v>
+        <v>109.128</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
@@ -3179,7 +3179,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>111448</v>
+        <v>111.44799999999999</v>
       </c>
       <c r="B49" t="s">
         <v>58</v>
@@ -3190,7 +3190,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>113750</v>
+        <v>113.75</v>
       </c>
       <c r="B50" t="s">
         <v>68</v>
@@ -3198,7 +3198,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>116093</v>
+        <v>116.093</v>
       </c>
       <c r="B51" t="s">
         <v>82</v>
@@ -3206,7 +3206,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>118422</v>
+        <v>118.422</v>
       </c>
       <c r="B52" t="s">
         <v>91</v>
@@ -3214,7 +3214,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>120761</v>
+        <v>120.761</v>
       </c>
       <c r="B53" t="s">
         <v>94</v>
@@ -3225,7 +3225,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>123077</v>
+        <v>123.077</v>
       </c>
       <c r="B54" t="s">
         <v>95</v>
@@ -3236,7 +3236,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>125384</v>
+        <v>125.384</v>
       </c>
       <c r="B55" t="s">
         <v>96</v>
@@ -3247,7 +3247,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>127698</v>
+        <v>127.69799999999999</v>
       </c>
       <c r="B56" t="s">
         <v>97</v>
@@ -3258,7 +3258,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>130012</v>
+        <v>130.012</v>
       </c>
       <c r="B57" t="s">
         <v>98</v>
@@ -3269,7 +3269,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>132316</v>
+        <v>132.316</v>
       </c>
       <c r="B58" t="s">
         <v>99</v>
@@ -3277,7 +3277,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>134653</v>
+        <v>134.65299999999999</v>
       </c>
       <c r="B59" t="s">
         <v>100</v>
@@ -3288,7 +3288,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>136964</v>
+        <v>136.964</v>
       </c>
       <c r="B60" t="s">
         <v>101</v>
@@ -3296,7 +3296,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>139294</v>
+        <v>139.29400000000001</v>
       </c>
       <c r="B61" t="s">
         <v>102</v>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>141604</v>
+        <v>141.60400000000001</v>
       </c>
       <c r="B62" t="s">
         <v>103</v>
@@ -3312,7 +3312,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>143924</v>
+        <v>143.92400000000001</v>
       </c>
       <c r="B63" t="s">
         <v>104</v>
@@ -3320,7 +3320,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>146246</v>
+        <v>146.24600000000001</v>
       </c>
       <c r="B64" t="s">
         <v>105</v>
@@ -3328,7 +3328,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>148566</v>
+        <v>148.566</v>
       </c>
       <c r="B65" t="s">
         <v>106</v>
@@ -3336,7 +3336,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>150864</v>
+        <v>150.864</v>
       </c>
       <c r="B66" t="s">
         <v>108</v>
@@ -3347,7 +3347,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>153172</v>
+        <v>153.172</v>
       </c>
       <c r="B67" t="s">
         <v>109</v>
@@ -3355,7 +3355,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>155513</v>
+        <v>155.51300000000001</v>
       </c>
       <c r="B68" t="s">
         <v>110</v>
@@ -3363,7 +3363,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>157814</v>
+        <v>157.81399999999999</v>
       </c>
       <c r="B69" t="s">
         <v>111</v>
@@ -3371,7 +3371,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>160126</v>
+        <v>160.126</v>
       </c>
       <c r="B70" t="s">
         <v>112</v>
@@ -3379,7 +3379,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>162424</v>
+        <v>162.42400000000001</v>
       </c>
       <c r="B71" t="s">
         <v>113</v>
@@ -3387,7 +3387,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>164719</v>
+        <v>164.71899999999999</v>
       </c>
       <c r="B72" t="s">
         <v>114</v>
@@ -3398,7 +3398,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>167044</v>
+        <v>167.04400000000001</v>
       </c>
       <c r="B73" t="s">
         <v>115</v>
@@ -3406,7 +3406,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>169117</v>
+        <v>169.11699999999999</v>
       </c>
       <c r="B74" t="s">
         <v>116</v>
@@ -3414,7 +3414,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>171421</v>
+        <v>171.42099999999999</v>
       </c>
       <c r="B75" t="s">
         <v>118</v>
@@ -3422,7 +3422,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>173975</v>
+        <v>173.97499999999999</v>
       </c>
       <c r="B76" t="s">
         <v>119</v>
@@ -3433,7 +3433,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>176288</v>
+        <v>176.28800000000001</v>
       </c>
       <c r="B77" t="s">
         <v>120</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>178588</v>
+        <v>178.58799999999999</v>
       </c>
       <c r="B78" t="s">
         <v>121</v>
@@ -3452,7 +3452,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>180912</v>
+        <v>180.91200000000001</v>
       </c>
       <c r="B79" t="s">
         <v>122</v>
@@ -3463,7 +3463,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>183199</v>
+        <v>183.19900000000001</v>
       </c>
       <c r="B80" t="s">
         <v>123</v>
@@ -3471,7 +3471,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>185523</v>
+        <v>185.523</v>
       </c>
       <c r="B81" t="s">
         <v>124</v>
@@ -3479,7 +3479,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>187839</v>
+        <v>187.839</v>
       </c>
       <c r="B82" t="s">
         <v>125</v>
@@ -3487,7 +3487,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>190132</v>
+        <v>190.13200000000001</v>
       </c>
       <c r="B83" t="s">
         <v>127</v>
@@ -3498,7 +3498,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>192433</v>
+        <v>192.43299999999999</v>
       </c>
       <c r="B84" t="s">
         <v>128</v>
@@ -3509,7 +3509,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>194751</v>
+        <v>194.751</v>
       </c>
       <c r="B85" t="s">
         <v>129</v>
@@ -3520,7 +3520,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>197093</v>
+        <v>197.09299999999999</v>
       </c>
       <c r="B86" t="s">
         <v>130</v>
@@ -3531,7 +3531,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>199435</v>
+        <v>199.435</v>
       </c>
       <c r="B87" t="s">
         <v>131</v>
@@ -3539,7 +3539,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>201751</v>
+        <v>201.751</v>
       </c>
       <c r="B88" t="s">
         <v>132</v>
@@ -3550,7 +3550,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>204053</v>
+        <v>204.053</v>
       </c>
       <c r="B89" t="s">
         <v>133</v>
@@ -3561,7 +3561,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>206372</v>
+        <v>206.37200000000001</v>
       </c>
       <c r="B90" t="s">
         <v>134</v>
@@ -3572,7 +3572,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>208677</v>
+        <v>208.67699999999999</v>
       </c>
       <c r="B91" t="s">
         <v>135</v>
@@ -3580,7 +3580,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>210992</v>
+        <v>210.99199999999999</v>
       </c>
       <c r="B92" t="s">
         <v>136</v>
@@ -3588,7 +3588,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>213303</v>
+        <v>213.303</v>
       </c>
       <c r="B93" t="s">
         <v>137</v>
@@ -3599,7 +3599,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>215620</v>
+        <v>215.62</v>
       </c>
       <c r="B94" t="s">
         <v>138</v>
@@ -3610,7 +3610,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>217960</v>
+        <v>217.96</v>
       </c>
       <c r="B95" t="s">
         <v>139</v>
@@ -3618,7 +3618,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>220394</v>
+        <v>220.39400000000001</v>
       </c>
       <c r="B96" t="s">
         <v>141</v>
@@ -3629,7 +3629,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>222572</v>
+        <v>222.572</v>
       </c>
       <c r="B97" t="s">
         <v>142</v>
@@ -3637,7 +3637,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>224907</v>
+        <v>224.90700000000001</v>
       </c>
       <c r="B98" t="s">
         <v>143</v>
@@ -3648,7 +3648,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>227230</v>
+        <v>227.23</v>
       </c>
       <c r="B99" t="s">
         <v>144</v>
@@ -3656,7 +3656,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>229530</v>
+        <v>229.53</v>
       </c>
       <c r="B100" t="s">
         <v>145</v>
@@ -3664,7 +3664,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>231821</v>
+        <v>231.821</v>
       </c>
       <c r="B101" t="s">
         <v>146</v>
@@ -3675,7 +3675,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>234100</v>
+        <v>234.1</v>
       </c>
       <c r="B102" t="s">
         <v>147</v>
@@ -3686,7 +3686,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>236433</v>
+        <v>236.43299999999999</v>
       </c>
       <c r="B103" t="s">
         <v>148</v>
@@ -3697,7 +3697,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>238748</v>
+        <v>238.74799999999999</v>
       </c>
       <c r="B104" t="s">
         <v>149</v>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>241316</v>
+        <v>241.316</v>
       </c>
       <c r="B105" t="s">
         <v>151</v>
@@ -3719,7 +3719,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>243630</v>
+        <v>243.63</v>
       </c>
       <c r="B106" t="s">
         <v>152</v>
@@ -3730,7 +3730,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>245932</v>
+        <v>245.93199999999999</v>
       </c>
       <c r="B107" t="s">
         <v>153</v>
@@ -3738,7 +3738,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>248263</v>
+        <v>248.26300000000001</v>
       </c>
       <c r="B108" t="s">
         <v>154</v>
@@ -3746,7 +3746,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>250582</v>
+        <v>250.58199999999999</v>
       </c>
       <c r="B109" t="s">
         <v>155</v>
@@ -3757,7 +3757,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>252897</v>
+        <v>252.89699999999999</v>
       </c>
       <c r="B110" t="s">
         <v>156</v>
@@ -3765,7 +3765,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>255190</v>
+        <v>255.19</v>
       </c>
       <c r="B111" t="s">
         <v>157</v>
@@ -3776,7 +3776,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>257492</v>
+        <v>257.49200000000002</v>
       </c>
       <c r="B112" t="s">
         <v>158</v>
@@ -3787,7 +3787,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>259794</v>
+        <v>259.79399999999998</v>
       </c>
       <c r="B113" t="s">
         <v>159</v>
@@ -3798,7 +3798,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>262112</v>
+        <v>262.11200000000002</v>
       </c>
       <c r="B114" t="s">
         <v>161</v>
@@ -3809,7 +3809,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>264432</v>
+        <v>264.43200000000002</v>
       </c>
       <c r="B115" t="s">
         <v>162</v>
@@ -3817,7 +3817,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>266768</v>
+        <v>266.76799999999997</v>
       </c>
       <c r="B116" t="s">
         <v>163</v>
@@ -3825,7 +3825,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>269062</v>
+        <v>269.06200000000001</v>
       </c>
       <c r="B117" t="s">
         <v>164</v>
@@ -3833,7 +3833,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>271372</v>
+        <v>271.37200000000001</v>
       </c>
       <c r="B118" t="s">
         <v>165</v>
@@ -3841,7 +3841,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>273701</v>
+        <v>273.70100000000002</v>
       </c>
       <c r="B119" t="s">
         <v>166</v>
@@ -3852,7 +3852,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>275997</v>
+        <v>275.99700000000001</v>
       </c>
       <c r="B120" t="s">
         <v>167</v>
@@ -3860,7 +3860,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>278327</v>
+        <v>278.327</v>
       </c>
       <c r="B121" t="s">
         <v>168</v>
@@ -3868,7 +3868,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>280642</v>
+        <v>280.642</v>
       </c>
       <c r="B122" t="s">
         <v>169</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>282963</v>
+        <v>282.96300000000002</v>
       </c>
       <c r="B123" t="s">
         <v>170</v>
@@ -3884,7 +3884,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>285303</v>
+        <v>285.303</v>
       </c>
       <c r="B124" t="s">
         <v>171</v>
@@ -3892,7 +3892,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>287609</v>
+        <v>287.60899999999998</v>
       </c>
       <c r="B125" t="s">
         <v>172</v>
@@ -3900,7 +3900,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>289922</v>
+        <v>289.92200000000003</v>
       </c>
       <c r="B126" t="s">
         <v>173</v>
@@ -3908,7 +3908,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>292273</v>
+        <v>292.27300000000002</v>
       </c>
       <c r="B127" t="s">
         <v>175</v>
@@ -3919,7 +3919,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>294582</v>
+        <v>294.58199999999999</v>
       </c>
       <c r="B128" t="s">
         <v>176</v>
@@ -3927,7 +3927,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>297049</v>
+        <v>297.04899999999998</v>
       </c>
       <c r="B129" t="s">
         <v>177</v>
@@ -3938,7 +3938,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>299212</v>
+        <v>299.21199999999999</v>
       </c>
       <c r="B130" t="s">
         <v>178</v>
@@ -3946,7 +3946,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>301522</v>
+        <v>301.52199999999999</v>
       </c>
       <c r="B131" t="s">
         <v>180</v>
@@ -3957,7 +3957,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>303842</v>
+        <v>303.84199999999998</v>
       </c>
       <c r="B132" t="s">
         <v>181</v>
@@ -3968,7 +3968,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>306153</v>
+        <v>306.15300000000002</v>
       </c>
       <c r="B133" t="s">
         <v>182</v>
@@ -3976,7 +3976,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>308467</v>
+        <v>308.46699999999998</v>
       </c>
       <c r="B134" t="s">
         <v>183</v>
@@ -3987,7 +3987,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>311026</v>
+        <v>311.02600000000001</v>
       </c>
       <c r="B135" t="s">
         <v>185</v>
@@ -3995,7 +3995,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>313316</v>
+        <v>313.31599999999997</v>
       </c>
       <c r="B136" t="s">
         <v>186</v>
@@ -4003,7 +4003,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>315612</v>
+        <v>315.61200000000002</v>
       </c>
       <c r="B137" t="s">
         <v>187</v>
@@ -4014,7 +4014,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>317929</v>
+        <v>317.92899999999997</v>
       </c>
       <c r="B138" t="s">
         <v>188</v>
@@ -4025,7 +4025,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>320218</v>
+        <v>320.21800000000002</v>
       </c>
       <c r="B139" t="s">
         <v>189</v>
@@ -4036,7 +4036,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>322532</v>
+        <v>322.53199999999998</v>
       </c>
       <c r="B140" t="s">
         <v>190</v>
@@ -4047,7 +4047,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>324832</v>
+        <v>324.83199999999999</v>
       </c>
       <c r="B141" t="s">
         <v>191</v>
@@ -4055,7 +4055,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>327172</v>
+        <v>327.17200000000003</v>
       </c>
       <c r="B142" t="s">
         <v>192</v>
@@ -4066,7 +4066,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143">
-        <v>329473</v>
+        <v>329.47300000000001</v>
       </c>
       <c r="B143" t="s">
         <v>193</v>
@@ -4074,7 +4074,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144">
-        <v>331787</v>
+        <v>331.78699999999998</v>
       </c>
       <c r="B144" t="s">
         <v>195</v>
@@ -4085,7 +4085,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145">
-        <v>334082</v>
+        <v>334.08199999999999</v>
       </c>
       <c r="B145" t="s">
         <v>196</v>
@@ -4096,7 +4096,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>336372</v>
+        <v>336.37200000000001</v>
       </c>
       <c r="B146" t="s">
         <v>197</v>
@@ -4107,7 +4107,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>338663</v>
+        <v>338.66300000000001</v>
       </c>
       <c r="B147" t="s">
         <v>198</v>
@@ -4118,7 +4118,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>340993</v>
+        <v>340.99299999999999</v>
       </c>
       <c r="B148" t="s">
         <v>199</v>
@@ -4129,7 +4129,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149">
-        <v>343314</v>
+        <v>343.31400000000002</v>
       </c>
       <c r="B149" t="s">
         <v>200</v>
@@ -4140,7 +4140,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150">
-        <v>345612</v>
+        <v>345.61200000000002</v>
       </c>
       <c r="B150" t="s">
         <v>201</v>
@@ -4151,7 +4151,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151">
-        <v>347952</v>
+        <v>347.952</v>
       </c>
       <c r="B151" t="s">
         <v>202</v>
@@ -4162,7 +4162,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152">
-        <v>350265</v>
+        <v>350.26499999999999</v>
       </c>
       <c r="B152" t="s">
         <v>203</v>
@@ -4170,7 +4170,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153">
-        <v>352572</v>
+        <v>352.572</v>
       </c>
       <c r="B153" t="s">
         <v>204</v>
@@ -4181,7 +4181,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154">
-        <v>354878</v>
+        <v>354.87799999999999</v>
       </c>
       <c r="B154" t="s">
         <v>205</v>
@@ -4192,7 +4192,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155">
-        <v>357202</v>
+        <v>357.202</v>
       </c>
       <c r="B155" t="s">
         <v>206</v>
@@ -4203,7 +4203,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156">
-        <v>359522</v>
+        <v>359.52199999999999</v>
       </c>
       <c r="B156" t="s">
         <v>207</v>
@@ -4214,7 +4214,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157">
-        <v>361812</v>
+        <v>361.81200000000001</v>
       </c>
       <c r="B157" t="s">
         <v>209</v>
@@ -4222,7 +4222,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>364143</v>
+        <v>364.14299999999997</v>
       </c>
       <c r="B158" t="s">
         <v>210</v>
@@ -4233,7 +4233,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159">
-        <v>366460</v>
+        <v>366.46</v>
       </c>
       <c r="B159" t="s">
         <v>211</v>
@@ -4241,7 +4241,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160">
-        <v>368803</v>
+        <v>368.803</v>
       </c>
       <c r="B160" t="s">
         <v>212</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161">
-        <v>371097</v>
+        <v>371.09699999999998</v>
       </c>
       <c r="B161" t="s">
         <v>213</v>
@@ -4263,7 +4263,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162">
-        <v>373391</v>
+        <v>373.39100000000002</v>
       </c>
       <c r="B162" t="s">
         <v>214</v>
@@ -4274,7 +4274,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163">
-        <v>375702</v>
+        <v>375.702</v>
       </c>
       <c r="B163" t="s">
         <v>215</v>
@@ -4282,7 +4282,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164">
-        <v>378033</v>
+        <v>378.03300000000002</v>
       </c>
       <c r="B164" t="s">
         <v>216</v>
@@ -4290,7 +4290,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165">
-        <v>380583</v>
+        <v>380.58300000000003</v>
       </c>
       <c r="B165" t="s">
         <v>218</v>
@@ -4298,7 +4298,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>382657</v>
+        <v>382.65699999999998</v>
       </c>
       <c r="B166" t="s">
         <v>219</v>
@@ -4309,7 +4309,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167">
-        <v>385215</v>
+        <v>385.21499999999997</v>
       </c>
       <c r="B167" t="s">
         <v>220</v>
@@ -4320,7 +4320,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168">
-        <v>387527</v>
+        <v>387.52699999999999</v>
       </c>
       <c r="B168" t="s">
         <v>221</v>
@@ -4331,7 +4331,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169">
-        <v>389844</v>
+        <v>389.84399999999999</v>
       </c>
       <c r="B169" t="s">
         <v>222</v>
@@ -4342,7 +4342,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>392182</v>
+        <v>392.18200000000002</v>
       </c>
       <c r="B170" t="s">
         <v>223</v>
@@ -4350,7 +4350,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171">
-        <v>394498</v>
+        <v>394.49799999999999</v>
       </c>
       <c r="B171" t="s">
         <v>224</v>
@@ -4358,7 +4358,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172">
-        <v>396821</v>
+        <v>396.82100000000003</v>
       </c>
       <c r="B172" t="s">
         <v>225</v>
@@ -4369,7 +4369,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173">
-        <v>398888</v>
+        <v>398.88799999999998</v>
       </c>
       <c r="B173" t="s">
         <v>226</v>
@@ -4377,7 +4377,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174">
-        <v>401212</v>
+        <v>401.21199999999999</v>
       </c>
       <c r="B174" t="s">
         <v>228</v>
@@ -4385,7 +4385,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175">
-        <v>403512</v>
+        <v>403.512</v>
       </c>
       <c r="B175" t="s">
         <v>229</v>
@@ -4393,7 +4393,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176">
-        <v>405850</v>
+        <v>405.85</v>
       </c>
       <c r="B176" t="s">
         <v>230</v>
@@ -4401,7 +4401,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>408162</v>
+        <v>408.16199999999998</v>
       </c>
       <c r="B177" t="s">
         <v>231</v>
@@ -4409,7 +4409,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>410504</v>
+        <v>410.50400000000002</v>
       </c>
       <c r="B178" t="s">
         <v>232</v>
@@ -4420,7 +4420,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179">
-        <v>412784</v>
+        <v>412.78399999999999</v>
       </c>
       <c r="B179" t="s">
         <v>233</v>
@@ -4431,7 +4431,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>415326</v>
+        <v>415.32600000000002</v>
       </c>
       <c r="B180" t="s">
         <v>234</v>
@@ -4439,7 +4439,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181">
-        <v>417622</v>
+        <v>417.62200000000001</v>
       </c>
       <c r="B181" t="s">
         <v>235</v>
@@ -4447,7 +4447,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182">
-        <v>419942</v>
+        <v>419.94200000000001</v>
       </c>
       <c r="B182" t="s">
         <v>236</v>
@@ -4458,7 +4458,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183">
-        <v>422272</v>
+        <v>422.27199999999999</v>
       </c>
       <c r="B183" t="s">
         <v>238</v>
@@ -4466,7 +4466,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184">
-        <v>424572</v>
+        <v>424.572</v>
       </c>
       <c r="B184" t="s">
         <v>239</v>
@@ -4474,7 +4474,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185">
-        <v>426882</v>
+        <v>426.88200000000001</v>
       </c>
       <c r="B185" t="s">
         <v>240</v>
@@ -4485,7 +4485,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186">
-        <v>429204</v>
+        <v>429.20400000000001</v>
       </c>
       <c r="B186" t="s">
         <v>241</v>
@@ -4493,7 +4493,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187">
-        <v>431512</v>
+        <v>431.512</v>
       </c>
       <c r="B187" t="s">
         <v>242</v>
@@ -4504,7 +4504,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188">
-        <v>433820</v>
+        <v>433.82</v>
       </c>
       <c r="B188" t="s">
         <v>243</v>
@@ -4512,7 +4512,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189">
-        <v>436142</v>
+        <v>436.142</v>
       </c>
       <c r="B189" t="s">
         <v>244</v>
@@ -4520,7 +4520,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190">
-        <v>438472</v>
+        <v>438.47199999999998</v>
       </c>
       <c r="B190" t="s">
         <v>245</v>
@@ -4531,7 +4531,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191">
-        <v>440792</v>
+        <v>440.79199999999997</v>
       </c>
       <c r="B191" t="s">
         <v>246</v>
@@ -4539,7 +4539,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192">
-        <v>443112</v>
+        <v>443.11200000000002</v>
       </c>
       <c r="B192" t="s">
         <v>247</v>
@@ -4547,7 +4547,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193">
-        <v>445442</v>
+        <v>445.44200000000001</v>
       </c>
       <c r="B193" t="s">
         <v>248</v>
@@ -4558,7 +4558,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194">
-        <v>447773</v>
+        <v>447.77300000000002</v>
       </c>
       <c r="B194" t="s">
         <v>249</v>
@@ -4566,7 +4566,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195">
-        <v>450116</v>
+        <v>450.11599999999999</v>
       </c>
       <c r="B195" t="s">
         <v>251</v>
@@ -4577,7 +4577,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196">
-        <v>452422</v>
+        <v>452.42200000000003</v>
       </c>
       <c r="B196" t="s">
         <v>252</v>
@@ -4588,7 +4588,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197">
-        <v>454731</v>
+        <v>454.73099999999999</v>
       </c>
       <c r="B197" t="s">
         <v>253</v>
@@ -4596,7 +4596,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198">
-        <v>457050</v>
+        <v>457.05</v>
       </c>
       <c r="B198" t="s">
         <v>254</v>
@@ -4604,7 +4604,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199">
-        <v>459358</v>
+        <v>459.358</v>
       </c>
       <c r="B199" t="s">
         <v>255</v>
@@ -4612,7 +4612,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200">
-        <v>461683</v>
+        <v>461.68299999999999</v>
       </c>
       <c r="B200" t="s">
         <v>256</v>
@@ -4623,7 +4623,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201">
-        <v>463994</v>
+        <v>463.99400000000003</v>
       </c>
       <c r="B201" t="s">
         <v>257</v>
@@ -4631,7 +4631,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202">
-        <v>466302</v>
+        <v>466.30200000000002</v>
       </c>
       <c r="B202" t="s">
         <v>258</v>
@@ -4639,7 +4639,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203">
-        <v>468612</v>
+        <v>468.61200000000002</v>
       </c>
       <c r="B203" t="s">
         <v>259</v>
@@ -4647,7 +4647,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204">
-        <v>470934</v>
+        <v>470.93400000000003</v>
       </c>
       <c r="B204" t="s">
         <v>261</v>
@@ -4655,7 +4655,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205">
-        <v>473273</v>
+        <v>473.27300000000002</v>
       </c>
       <c r="B205" t="s">
         <v>262</v>
@@ -4666,7 +4666,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206">
-        <v>475573</v>
+        <v>475.57299999999998</v>
       </c>
       <c r="B206" t="s">
         <v>263</v>
@@ -4677,7 +4677,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207">
-        <v>477889</v>
+        <v>477.88900000000001</v>
       </c>
       <c r="B207" t="s">
         <v>264</v>
@@ -4685,7 +4685,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208">
-        <v>480212</v>
+        <v>480.21199999999999</v>
       </c>
       <c r="B208" t="s">
         <v>265</v>
@@ -4696,7 +4696,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209">
-        <v>482542</v>
+        <v>482.54199999999997</v>
       </c>
       <c r="B209" t="s">
         <v>266</v>
@@ -4704,7 +4704,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210">
-        <v>484835</v>
+        <v>484.83499999999998</v>
       </c>
       <c r="B210" t="s">
         <v>267</v>
@@ -4715,7 +4715,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211">
-        <v>487142</v>
+        <v>487.142</v>
       </c>
       <c r="B211" t="s">
         <v>268</v>
@@ -4726,7 +4726,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212">
-        <v>489452</v>
+        <v>489.452</v>
       </c>
       <c r="B212" t="s">
         <v>269</v>
@@ -4737,7 +4737,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213">
-        <v>491772</v>
+        <v>491.77199999999999</v>
       </c>
       <c r="B213" t="s">
         <v>271</v>
@@ -4745,7 +4745,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214">
-        <v>494100</v>
+        <v>494.1</v>
       </c>
       <c r="B214" t="s">
         <v>272</v>
@@ -4756,7 +4756,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215">
-        <v>496407</v>
+        <v>496.40699999999998</v>
       </c>
       <c r="B215" t="s">
         <v>273</v>
@@ -4764,7 +4764,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216">
-        <v>498722</v>
+        <v>498.72199999999998</v>
       </c>
       <c r="B216" t="s">
         <v>274</v>
@@ -4775,7 +4775,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217">
-        <v>501031</v>
+        <v>501.03100000000001</v>
       </c>
       <c r="B217" t="s">
         <v>276</v>
@@ -4783,7 +4783,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218">
-        <v>503341</v>
+        <v>503.34100000000001</v>
       </c>
       <c r="B218" t="s">
         <v>277</v>
@@ -4794,7 +4794,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219">
-        <v>505672</v>
+        <v>505.67200000000003</v>
       </c>
       <c r="B219" t="s">
         <v>278</v>
@@ -4802,7 +4802,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220">
-        <v>507993</v>
+        <v>507.99299999999999</v>
       </c>
       <c r="B220" t="s">
         <v>279</v>
@@ -4813,7 +4813,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221">
-        <v>510293</v>
+        <v>510.29300000000001</v>
       </c>
       <c r="B221" t="s">
         <v>280</v>
@@ -4824,7 +4824,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222">
-        <v>512622</v>
+        <v>512.62199999999996</v>
       </c>
       <c r="B222" t="s">
         <v>281</v>
@@ -4832,7 +4832,7 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223">
-        <v>514952</v>
+        <v>514.952</v>
       </c>
       <c r="B223" t="s">
         <v>282</v>
@@ -4843,7 +4843,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224">
-        <v>517283</v>
+        <v>517.28300000000002</v>
       </c>
       <c r="B224" t="s">
         <v>283</v>
@@ -4851,7 +4851,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225">
-        <v>519602</v>
+        <v>519.60199999999998</v>
       </c>
       <c r="B225" t="s">
         <v>284</v>
@@ -4862,7 +4862,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226">
-        <v>521897</v>
+        <v>521.89700000000005</v>
       </c>
       <c r="B226" t="s">
         <v>286</v>
@@ -4870,7 +4870,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227">
-        <v>524212</v>
+        <v>524.21199999999999</v>
       </c>
       <c r="B227" t="s">
         <v>287</v>
@@ -4881,7 +4881,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228">
-        <v>526523</v>
+        <v>526.52300000000002</v>
       </c>
       <c r="B228" t="s">
         <v>288</v>
@@ -4889,7 +4889,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229">
-        <v>529057</v>
+        <v>529.05700000000002</v>
       </c>
       <c r="B229" t="s">
         <v>289</v>
@@ -4897,7 +4897,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230">
-        <v>531212</v>
+        <v>531.21199999999999</v>
       </c>
       <c r="B230" t="s">
         <v>290</v>
@@ -4908,7 +4908,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231">
-        <v>533520</v>
+        <v>533.52</v>
       </c>
       <c r="B231" t="s">
         <v>291</v>
@@ -4919,7 +4919,7 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232">
-        <v>535827</v>
+        <v>535.827</v>
       </c>
       <c r="B232" t="s">
         <v>292</v>
@@ -4930,7 +4930,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233">
-        <v>538152</v>
+        <v>538.15200000000004</v>
       </c>
       <c r="B233" t="s">
         <v>293</v>
@@ -4941,7 +4941,7 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234">
-        <v>540461</v>
+        <v>540.46100000000001</v>
       </c>
       <c r="B234" t="s">
         <v>295</v>
@@ -4952,7 +4952,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235">
-        <v>542777</v>
+        <v>542.77700000000004</v>
       </c>
       <c r="B235" t="s">
         <v>296</v>
@@ -4963,7 +4963,7 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236">
-        <v>545082</v>
+        <v>545.08199999999999</v>
       </c>
       <c r="B236" t="s">
         <v>297</v>
@@ -4971,7 +4971,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237">
-        <v>547381</v>
+        <v>547.38099999999997</v>
       </c>
       <c r="B237" t="s">
         <v>298</v>
@@ -4982,7 +4982,7 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238">
-        <v>549932</v>
+        <v>549.93200000000002</v>
       </c>
       <c r="B238" t="s">
         <v>299</v>
@@ -4993,7 +4993,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239">
-        <v>552224</v>
+        <v>552.22400000000005</v>
       </c>
       <c r="B239" t="s">
         <v>300</v>
@@ -5004,7 +5004,7 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240">
-        <v>554536</v>
+        <v>554.53599999999994</v>
       </c>
       <c r="B240" t="s">
         <v>301</v>
@@ -5012,7 +5012,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241">
-        <v>556830</v>
+        <v>556.83000000000004</v>
       </c>
       <c r="B241" t="s">
         <v>302</v>
@@ -5023,7 +5023,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242">
-        <v>559132</v>
+        <v>559.13199999999995</v>
       </c>
       <c r="B242" t="s">
         <v>303</v>
@@ -5031,7 +5031,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243">
-        <v>561482</v>
+        <v>561.48199999999997</v>
       </c>
       <c r="B243" t="s">
         <v>305</v>
@@ -5039,7 +5039,7 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244">
-        <v>563823</v>
+        <v>563.82299999999998</v>
       </c>
       <c r="B244" t="s">
         <v>306</v>
@@ -5050,7 +5050,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245">
-        <v>566112</v>
+        <v>566.11199999999997</v>
       </c>
       <c r="B245" t="s">
         <v>307</v>
@@ -5058,7 +5058,7 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246">
-        <v>568407</v>
+        <v>568.40700000000004</v>
       </c>
       <c r="B246" t="s">
         <v>308</v>
@@ -5066,7 +5066,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247">
-        <v>570725</v>
+        <v>570.72500000000002</v>
       </c>
       <c r="B247" t="s">
         <v>309</v>
@@ -5074,7 +5074,7 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248">
-        <v>573042</v>
+        <v>573.04200000000003</v>
       </c>
       <c r="B248" t="s">
         <v>310</v>
@@ -5082,7 +5082,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249">
-        <v>575382</v>
+        <v>575.38199999999995</v>
       </c>
       <c r="B249" t="s">
         <v>311</v>
@@ -5090,7 +5090,7 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250">
-        <v>577722</v>
+        <v>577.72199999999998</v>
       </c>
       <c r="B250" t="s">
         <v>312</v>
@@ -5101,7 +5101,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251">
-        <v>580038</v>
+        <v>580.03800000000001</v>
       </c>
       <c r="B251" t="s">
         <v>313</v>
@@ -5112,7 +5112,7 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252">
-        <v>582344</v>
+        <v>582.34400000000005</v>
       </c>
       <c r="B252" t="s">
         <v>314</v>
@@ -5123,7 +5123,7 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253">
-        <v>584671</v>
+        <v>584.67100000000005</v>
       </c>
       <c r="B253" t="s">
         <v>315</v>
@@ -5131,7 +5131,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254">
-        <v>586995</v>
+        <v>586.995</v>
       </c>
       <c r="B254" t="s">
         <v>316</v>
@@ -5142,7 +5142,7 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255">
-        <v>589292</v>
+        <v>589.29200000000003</v>
       </c>
       <c r="B255" t="s">
         <v>317</v>
@@ -5153,7 +5153,7 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256">
-        <v>591356</v>
+        <v>591.35599999999999</v>
       </c>
       <c r="B256" t="s">
         <v>319</v>
@@ -5161,7 +5161,7 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257">
-        <v>593662</v>
+        <v>593.66200000000003</v>
       </c>
       <c r="B257" t="s">
         <v>320</v>
@@ -5172,7 +5172,7 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258">
-        <v>596091</v>
+        <v>596.09100000000001</v>
       </c>
       <c r="B258" t="s">
         <v>321</v>
@@ -5180,7 +5180,7 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259">
-        <v>598282</v>
+        <v>598.28200000000004</v>
       </c>
       <c r="B259" t="s">
         <v>322</v>
@@ -5188,7 +5188,7 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260">
-        <v>600592</v>
+        <v>600.59199999999998</v>
       </c>
       <c r="B260" t="s">
         <v>323</v>
@@ -5199,7 +5199,7 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261">
-        <v>603160</v>
+        <v>603.16</v>
       </c>
       <c r="B261" t="s">
         <v>324</v>
@@ -5210,7 +5210,7 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262">
-        <v>605452</v>
+        <v>605.452</v>
       </c>
       <c r="B262" t="s">
         <v>325</v>
@@ -5221,7 +5221,7 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263">
-        <v>607775</v>
+        <v>607.77499999999998</v>
       </c>
       <c r="B263" t="s">
         <v>326</v>
@@ -5232,7 +5232,7 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264">
-        <v>610078</v>
+        <v>610.07799999999997</v>
       </c>
       <c r="B264" t="s">
         <v>328</v>
@@ -5240,7 +5240,7 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265">
-        <v>612429</v>
+        <v>612.42899999999997</v>
       </c>
       <c r="B265" t="s">
         <v>329</v>
@@ -5248,7 +5248,7 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266">
-        <v>614724</v>
+        <v>614.72400000000005</v>
       </c>
       <c r="B266" t="s">
         <v>330</v>
@@ -5259,7 +5259,7 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267">
-        <v>617017</v>
+        <v>617.01700000000005</v>
       </c>
       <c r="B267" t="s">
         <v>331</v>
@@ -5270,7 +5270,7 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268">
-        <v>619340</v>
+        <v>619.34</v>
       </c>
       <c r="B268" t="s">
         <v>332</v>
@@ -5281,7 +5281,7 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269">
-        <v>621665</v>
+        <v>621.66499999999996</v>
       </c>
       <c r="B269" t="s">
         <v>333</v>
@@ -5289,7 +5289,7 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270">
-        <v>623973</v>
+        <v>623.97299999999996</v>
       </c>
       <c r="B270" t="s">
         <v>334</v>
@@ -5297,7 +5297,7 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271">
-        <v>626296</v>
+        <v>626.29600000000005</v>
       </c>
       <c r="B271" t="s">
         <v>335</v>
@@ -5305,7 +5305,7 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272">
-        <v>628598</v>
+        <v>628.59799999999996</v>
       </c>
       <c r="B272" t="s">
         <v>336</v>
@@ -5313,7 +5313,7 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273">
-        <v>630895</v>
+        <v>630.89499999999998</v>
       </c>
       <c r="B273" t="s">
         <v>338</v>
@@ -5321,7 +5321,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274">
-        <v>633200</v>
+        <v>633.20000000000005</v>
       </c>
       <c r="B274" t="s">
         <v>339</v>
@@ -5329,7 +5329,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275">
-        <v>635523</v>
+        <v>635.52300000000002</v>
       </c>
       <c r="B275" t="s">
         <v>340</v>
@@ -5337,7 +5337,7 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276">
-        <v>637816</v>
+        <v>637.81600000000003</v>
       </c>
       <c r="B276" t="s">
         <v>341</v>
@@ -5348,7 +5348,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277">
-        <v>640135</v>
+        <v>640.13499999999999</v>
       </c>
       <c r="B277" t="s">
         <v>342</v>
@@ -5359,7 +5359,7 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278">
-        <v>642194</v>
+        <v>642.19399999999996</v>
       </c>
       <c r="B278" t="s">
         <v>343</v>
@@ -5367,7 +5367,7 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279">
-        <v>644512</v>
+        <v>644.51199999999994</v>
       </c>
       <c r="B279" t="s">
         <v>344</v>
@@ -5375,7 +5375,7 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280">
-        <v>647073</v>
+        <v>647.07299999999998</v>
       </c>
       <c r="B280" t="s">
         <v>345</v>
@@ -5383,7 +5383,7 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281">
-        <v>649352</v>
+        <v>649.35199999999998</v>
       </c>
       <c r="B281" t="s">
         <v>346</v>
@@ -5394,7 +5394,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282">
-        <v>651679</v>
+        <v>651.67899999999997</v>
       </c>
       <c r="B282" t="s">
         <v>347</v>
@@ -5405,7 +5405,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283">
-        <v>653979</v>
+        <v>653.97900000000004</v>
       </c>
       <c r="B283" t="s">
         <v>348</v>
@@ -5413,7 +5413,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284">
-        <v>656294</v>
+        <v>656.29399999999998</v>
       </c>
       <c r="B284" t="s">
         <v>349</v>
@@ -5421,7 +5421,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285">
-        <v>658378</v>
+        <v>658.37800000000004</v>
       </c>
       <c r="B285" t="s">
         <v>350</v>
@@ -5429,7 +5429,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286">
-        <v>660692</v>
+        <v>660.69200000000001</v>
       </c>
       <c r="B286" t="s">
         <v>352</v>
@@ -5437,7 +5437,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287">
-        <v>663003</v>
+        <v>663.00300000000004</v>
       </c>
       <c r="B287" t="s">
         <v>353</v>
@@ -5448,7 +5448,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288">
-        <v>665577</v>
+        <v>665.577</v>
       </c>
       <c r="B288" t="s">
         <v>354</v>
@@ -5459,7 +5459,7 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289">
-        <v>667882</v>
+        <v>667.88199999999995</v>
       </c>
       <c r="B289" t="s">
         <v>355</v>
@@ -5467,7 +5467,7 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290">
-        <v>670183</v>
+        <v>670.18299999999999</v>
       </c>
       <c r="B290" t="s">
         <v>356</v>
@@ -5478,7 +5478,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291">
-        <v>672501</v>
+        <v>672.50099999999998</v>
       </c>
       <c r="B291" t="s">
         <v>357</v>
@@ -5489,7 +5489,7 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292">
-        <v>674811</v>
+        <v>674.81100000000004</v>
       </c>
       <c r="B292" t="s">
         <v>358</v>
@@ -5497,7 +5497,7 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293">
-        <v>676872</v>
+        <v>676.87199999999996</v>
       </c>
       <c r="B293" t="s">
         <v>359</v>
@@ -5508,7 +5508,7 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294">
-        <v>679443</v>
+        <v>679.44299999999998</v>
       </c>
       <c r="B294" t="s">
         <v>360</v>
@@ -5516,7 +5516,7 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295">
-        <v>681735</v>
+        <v>681.73500000000001</v>
       </c>
       <c r="B295" t="s">
         <v>362</v>
@@ -5527,7 +5527,7 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296">
-        <v>683803</v>
+        <v>683.803</v>
       </c>
       <c r="B296" t="s">
         <v>363</v>
@@ -5535,7 +5535,7 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297">
-        <v>686352</v>
+        <v>686.35199999999998</v>
       </c>
       <c r="B297" t="s">
         <v>364</v>
@@ -5543,7 +5543,7 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298">
-        <v>688675</v>
+        <v>688.67499999999995</v>
       </c>
       <c r="B298" t="s">
         <v>365</v>
@@ -5551,7 +5551,7 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299">
-        <v>690973</v>
+        <v>690.97299999999996</v>
       </c>
       <c r="B299" t="s">
         <v>366</v>
@@ -5562,7 +5562,7 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300">
-        <v>693285</v>
+        <v>693.28499999999997</v>
       </c>
       <c r="B300" t="s">
         <v>367</v>
@@ -5573,7 +5573,7 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301">
-        <v>695601</v>
+        <v>695.601</v>
       </c>
       <c r="B301" t="s">
         <v>368</v>
@@ -5584,7 +5584,7 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302">
-        <v>697876</v>
+        <v>697.87599999999998</v>
       </c>
       <c r="B302" t="s">
         <v>369</v>
@@ -5592,7 +5592,7 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A303">
-        <v>700191</v>
+        <v>700.19100000000003</v>
       </c>
       <c r="B303" t="s">
         <v>371</v>
@@ -5603,7 +5603,7 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304">
-        <v>702507</v>
+        <v>702.50699999999995</v>
       </c>
       <c r="B304" t="s">
         <v>372</v>
@@ -5614,7 +5614,7 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A305">
-        <v>704820</v>
+        <v>704.82</v>
       </c>
       <c r="B305" t="s">
         <v>373</v>
@@ -5625,7 +5625,7 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A306">
-        <v>707112</v>
+        <v>707.11199999999997</v>
       </c>
       <c r="B306" t="s">
         <v>374</v>
@@ -5636,7 +5636,7 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307">
-        <v>709442</v>
+        <v>709.44200000000001</v>
       </c>
       <c r="B307" t="s">
         <v>375</v>
@@ -5647,7 +5647,7 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308">
-        <v>711752</v>
+        <v>711.75199999999995</v>
       </c>
       <c r="B308" t="s">
         <v>376</v>
@@ -5655,7 +5655,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309">
-        <v>714076</v>
+        <v>714.07600000000002</v>
       </c>
       <c r="B309" t="s">
         <v>377</v>
@@ -5666,7 +5666,7 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A310">
-        <v>716402</v>
+        <v>716.40200000000004</v>
       </c>
       <c r="B310" t="s">
         <v>378</v>
@@ -5677,7 +5677,7 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A311">
-        <v>718712</v>
+        <v>718.71199999999999</v>
       </c>
       <c r="B311" t="s">
         <v>379</v>
@@ -5688,7 +5688,7 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A312">
-        <v>721049</v>
+        <v>721.04899999999998</v>
       </c>
       <c r="B312" t="s">
         <v>380</v>
@@ -5699,7 +5699,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313">
-        <v>723377</v>
+        <v>723.37699999999995</v>
       </c>
       <c r="B313" t="s">
         <v>381</v>
@@ -5710,7 +5710,7 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A314">
-        <v>725698</v>
+        <v>725.69799999999998</v>
       </c>
       <c r="B314" t="s">
         <v>382</v>
@@ -5721,7 +5721,7 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A315">
-        <v>728020</v>
+        <v>728.02</v>
       </c>
       <c r="B315" t="s">
         <v>383</v>
@@ -5732,7 +5732,7 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A316">
-        <v>730325</v>
+        <v>730.32500000000005</v>
       </c>
       <c r="B316" t="s">
         <v>385</v>
@@ -5743,7 +5743,7 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A317">
-        <v>732616</v>
+        <v>732.61599999999999</v>
       </c>
       <c r="B317" t="s">
         <v>386</v>
@@ -5751,7 +5751,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318">
-        <v>734933</v>
+        <v>734.93299999999999</v>
       </c>
       <c r="B318" t="s">
         <v>387</v>
@@ -5759,7 +5759,7 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A319">
-        <v>737240</v>
+        <v>737.24</v>
       </c>
       <c r="B319" t="s">
         <v>388</v>
@@ -5767,7 +5767,7 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A320">
-        <v>739542</v>
+        <v>739.54200000000003</v>
       </c>
       <c r="B320" t="s">
         <v>389</v>
@@ -5775,7 +5775,7 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A321">
-        <v>741871</v>
+        <v>741.87099999999998</v>
       </c>
       <c r="B321" t="s">
         <v>390</v>
@@ -5786,7 +5786,7 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A322">
-        <v>744167</v>
+        <v>744.16700000000003</v>
       </c>
       <c r="B322" t="s">
         <v>391</v>
@@ -5797,7 +5797,7 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A323">
-        <v>746473</v>
+        <v>746.47299999999996</v>
       </c>
       <c r="B323" t="s">
         <v>392</v>
@@ -5808,7 +5808,7 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A324">
-        <v>748802</v>
+        <v>748.80200000000002</v>
       </c>
       <c r="B324" t="s">
         <v>393</v>
@@ -5816,7 +5816,7 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A325">
-        <v>751113</v>
+        <v>751.11300000000006</v>
       </c>
       <c r="B325" t="s">
         <v>395</v>
@@ -5827,7 +5827,7 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A326">
-        <v>753433</v>
+        <v>753.43299999999999</v>
       </c>
       <c r="B326" t="s">
         <v>396</v>
@@ -5835,7 +5835,7 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A327">
-        <v>755743</v>
+        <v>755.74300000000005</v>
       </c>
       <c r="B327" t="s">
         <v>397</v>
@@ -5846,7 +5846,7 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A328">
-        <v>758065</v>
+        <v>758.06500000000005</v>
       </c>
       <c r="B328" t="s">
         <v>398</v>
@@ -5857,7 +5857,7 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A329">
-        <v>760392</v>
+        <v>760.39200000000005</v>
       </c>
       <c r="B329" t="s">
         <v>399</v>
@@ -5868,7 +5868,7 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A330">
-        <v>762714</v>
+        <v>762.71400000000006</v>
       </c>
       <c r="B330" t="s">
         <v>400</v>
@@ -5879,7 +5879,7 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A331">
-        <v>765072</v>
+        <v>765.072</v>
       </c>
       <c r="B331" t="s">
         <v>401</v>
@@ -5890,7 +5890,7 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332">
-        <v>767373</v>
+        <v>767.37300000000005</v>
       </c>
       <c r="B332" t="s">
         <v>402</v>
@@ -5901,7 +5901,7 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A333">
-        <v>769441</v>
+        <v>769.44100000000003</v>
       </c>
       <c r="B333" t="s">
         <v>403</v>
@@ -5912,7 +5912,7 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A334">
-        <v>772000</v>
+        <v>772</v>
       </c>
       <c r="B334" t="s">
         <v>405</v>
@@ -5923,7 +5923,7 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A335">
-        <v>774287</v>
+        <v>774.28700000000003</v>
       </c>
       <c r="B335" t="s">
         <v>406</v>
@@ -5934,7 +5934,7 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A336">
-        <v>776590</v>
+        <v>776.59</v>
       </c>
       <c r="B336" t="s">
         <v>407</v>
@@ -5942,7 +5942,7 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337">
-        <v>778908</v>
+        <v>778.90800000000002</v>
       </c>
       <c r="B337" t="s">
         <v>408</v>
@@ -5950,7 +5950,7 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338">
-        <v>781223</v>
+        <v>781.22299999999996</v>
       </c>
       <c r="B338" t="s">
         <v>409</v>
@@ -5961,7 +5961,7 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339">
-        <v>783542</v>
+        <v>783.54200000000003</v>
       </c>
       <c r="B339" t="s">
         <v>410</v>
@@ -5972,7 +5972,7 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340">
-        <v>785732</v>
+        <v>785.73199999999997</v>
       </c>
       <c r="B340" t="s">
         <v>411</v>
@@ -5983,7 +5983,7 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A341">
-        <v>788042</v>
+        <v>788.04200000000003</v>
       </c>
       <c r="B341" t="s">
         <v>412</v>
@@ -5991,7 +5991,7 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A342">
-        <v>790494</v>
+        <v>790.49400000000003</v>
       </c>
       <c r="B342" t="s">
         <v>414</v>
@@ -5999,7 +5999,7 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343">
-        <v>792670</v>
+        <v>792.67</v>
       </c>
       <c r="B343" t="s">
         <v>415</v>
@@ -6010,7 +6010,7 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A344">
-        <v>794982</v>
+        <v>794.98199999999997</v>
       </c>
       <c r="B344" t="s">
         <v>416</v>
@@ -6021,7 +6021,7 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A345">
-        <v>797299</v>
+        <v>797.29899999999998</v>
       </c>
       <c r="B345" t="s">
         <v>417</v>
@@ -6032,7 +6032,7 @@
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A346">
-        <v>799626</v>
+        <v>799.62599999999998</v>
       </c>
       <c r="B346" t="s">
         <v>418</v>
@@ -6043,7 +6043,7 @@
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A347">
-        <v>801927</v>
+        <v>801.92700000000002</v>
       </c>
       <c r="B347" t="s">
         <v>420</v>
@@ -6054,7 +6054,7 @@
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A348">
-        <v>804017</v>
+        <v>804.01700000000005</v>
       </c>
       <c r="B348" t="s">
         <v>421</v>
@@ -6065,7 +6065,7 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A349">
-        <v>806323</v>
+        <v>806.32299999999998</v>
       </c>
       <c r="B349" t="s">
         <v>422</v>
@@ -6076,7 +6076,7 @@
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A350">
-        <v>808652</v>
+        <v>808.65200000000004</v>
       </c>
       <c r="B350" t="s">
         <v>423</v>
@@ -6084,7 +6084,7 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A351">
-        <v>810962</v>
+        <v>810.96199999999999</v>
       </c>
       <c r="B351" t="s">
         <v>424</v>
@@ -6095,7 +6095,7 @@
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A352">
-        <v>813268</v>
+        <v>813.26800000000003</v>
       </c>
       <c r="B352" t="s">
         <v>425</v>
@@ -6106,7 +6106,7 @@
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A353">
-        <v>815581</v>
+        <v>815.58100000000002</v>
       </c>
       <c r="B353" t="s">
         <v>426</v>
@@ -6117,7 +6117,7 @@
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A354">
-        <v>817892</v>
+        <v>817.89200000000005</v>
       </c>
       <c r="B354" t="s">
         <v>427</v>
@@ -6125,7 +6125,7 @@
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A355">
-        <v>820206</v>
+        <v>820.20600000000002</v>
       </c>
       <c r="B355" t="s">
         <v>429</v>
@@ -6133,7 +6133,7 @@
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A356">
-        <v>822553</v>
+        <v>822.553</v>
       </c>
       <c r="B356" t="s">
         <v>430</v>
@@ -6141,7 +6141,7 @@
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A357">
-        <v>824871</v>
+        <v>824.87099999999998</v>
       </c>
       <c r="B357" t="s">
         <v>431</v>
@@ -6149,7 +6149,7 @@
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A358">
-        <v>827184</v>
+        <v>827.18399999999997</v>
       </c>
       <c r="B358" t="s">
         <v>432</v>
@@ -6157,7 +6157,7 @@
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A359">
-        <v>829220</v>
+        <v>829.22</v>
       </c>
       <c r="B359" t="s">
         <v>433</v>
@@ -6165,7 +6165,7 @@
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A360">
-        <v>831539</v>
+        <v>831.53899999999999</v>
       </c>
       <c r="B360" t="s">
         <v>434</v>
@@ -6176,7 +6176,7 @@
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A361">
-        <v>833860</v>
+        <v>833.86</v>
       </c>
       <c r="B361" t="s">
         <v>435</v>
@@ -6184,7 +6184,7 @@
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A362">
-        <v>836170</v>
+        <v>836.17</v>
       </c>
       <c r="B362" t="s">
         <v>436</v>
@@ -6192,7 +6192,7 @@
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A363">
-        <v>838492</v>
+        <v>838.49199999999996</v>
       </c>
       <c r="B363" t="s">
         <v>437</v>
@@ -6203,7 +6203,7 @@
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A364">
-        <v>840793</v>
+        <v>840.79300000000001</v>
       </c>
       <c r="B364" t="s">
         <v>439</v>
@@ -6214,7 +6214,7 @@
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A365">
-        <v>843103</v>
+        <v>843.10299999999995</v>
       </c>
       <c r="B365" t="s">
         <v>440</v>
@@ -6225,7 +6225,7 @@
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A366">
-        <v>845402</v>
+        <v>845.40200000000004</v>
       </c>
       <c r="B366" t="s">
         <v>441</v>
@@ -6236,7 +6236,7 @@
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A367">
-        <v>847713</v>
+        <v>847.71299999999997</v>
       </c>
       <c r="B367" t="s">
         <v>442</v>
@@ -6247,7 +6247,7 @@
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A368">
-        <v>849782</v>
+        <v>849.78200000000004</v>
       </c>
       <c r="B368" t="s">
         <v>443</v>
@@ -6258,7 +6258,7 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A369">
-        <v>852106</v>
+        <v>852.10599999999999</v>
       </c>
       <c r="B369" t="s">
         <v>444</v>
@@ -6269,7 +6269,7 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A370">
-        <v>854423</v>
+        <v>854.423</v>
       </c>
       <c r="B370" t="s">
         <v>445</v>
@@ -6280,7 +6280,7 @@
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A371">
-        <v>856722</v>
+        <v>856.72199999999998</v>
       </c>
       <c r="B371" t="s">
         <v>446</v>
@@ -6291,7 +6291,7 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A372">
-        <v>859022</v>
+        <v>859.02200000000005</v>
       </c>
       <c r="B372" t="s">
         <v>447</v>
@@ -6302,7 +6302,7 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A373">
-        <v>861344</v>
+        <v>861.34400000000005</v>
       </c>
       <c r="B373" t="s">
         <v>449</v>
@@ -6313,7 +6313,7 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A374">
-        <v>863642</v>
+        <v>863.64200000000005</v>
       </c>
       <c r="B374" t="s">
         <v>450</v>
@@ -6324,7 +6324,7 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A375">
-        <v>865962</v>
+        <v>865.96199999999999</v>
       </c>
       <c r="B375" t="s">
         <v>451</v>
@@ -6335,7 +6335,7 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A376">
-        <v>868315</v>
+        <v>868.31500000000005</v>
       </c>
       <c r="B376" t="s">
         <v>452</v>
@@ -6346,7 +6346,7 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A377">
-        <v>870614</v>
+        <v>870.61400000000003</v>
       </c>
       <c r="B377" t="s">
         <v>453</v>
@@ -6357,7 +6357,7 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A378">
-        <v>872673</v>
+        <v>872.673</v>
       </c>
       <c r="B378" t="s">
         <v>454</v>
@@ -6368,7 +6368,7 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A379">
-        <v>874992</v>
+        <v>874.99199999999996</v>
       </c>
       <c r="B379" t="s">
         <v>455</v>
@@ -6376,7 +6376,7 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A380">
-        <v>877302</v>
+        <v>877.30200000000002</v>
       </c>
       <c r="B380" t="s">
         <v>456</v>
@@ -6384,7 +6384,7 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A381">
-        <v>879620</v>
+        <v>879.62</v>
       </c>
       <c r="B381" t="s">
         <v>457</v>
@@ -6395,7 +6395,7 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A382">
-        <v>881933</v>
+        <v>881.93299999999999</v>
       </c>
       <c r="B382" t="s">
         <v>458</v>
@@ -6406,7 +6406,7 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A383">
-        <v>884231</v>
+        <v>884.23099999999999</v>
       </c>
       <c r="B383" t="s">
         <v>459</v>
@@ -6414,7 +6414,7 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A384">
-        <v>886550</v>
+        <v>886.55</v>
       </c>
       <c r="B384" t="s">
         <v>460</v>
@@ -6422,7 +6422,7 @@
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A385">
-        <v>888851</v>
+        <v>888.851</v>
       </c>
       <c r="B385" t="s">
         <v>461</v>
@@ -6433,7 +6433,7 @@
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A386">
-        <v>891167</v>
+        <v>891.16700000000003</v>
       </c>
       <c r="B386" t="s">
         <v>463</v>
@@ -6441,7 +6441,7 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A387">
-        <v>893464</v>
+        <v>893.46400000000006</v>
       </c>
       <c r="B387" t="s">
         <v>464</v>
@@ -6452,7 +6452,7 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A388">
-        <v>895793</v>
+        <v>895.79300000000001</v>
       </c>
       <c r="B388" t="s">
         <v>465</v>
@@ -6460,7 +6460,7 @@
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A389">
-        <v>898093</v>
+        <v>898.09299999999996</v>
       </c>
       <c r="B389" t="s">
         <v>466</v>
@@ -6471,7 +6471,7 @@
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A390">
-        <v>900410</v>
+        <v>900.41</v>
       </c>
       <c r="B390" t="s">
         <v>467</v>
@@ -6479,7 +6479,7 @@
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A391">
-        <v>902739</v>
+        <v>902.73900000000003</v>
       </c>
       <c r="B391" t="s">
         <v>468</v>
@@ -6490,7 +6490,7 @@
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A392">
-        <v>905040</v>
+        <v>905.04</v>
       </c>
       <c r="B392" t="s">
         <v>469</v>
@@ -6498,7 +6498,7 @@
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A393">
-        <v>907092</v>
+        <v>907.09199999999998</v>
       </c>
       <c r="B393" t="s">
         <v>470</v>
@@ -6509,7 +6509,7 @@
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A394">
-        <v>909392</v>
+        <v>909.39200000000005</v>
       </c>
       <c r="B394" t="s">
         <v>471</v>
@@ -6520,7 +6520,7 @@
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A395">
-        <v>911682</v>
+        <v>911.68200000000002</v>
       </c>
       <c r="B395" t="s">
         <v>473</v>
@@ -6531,7 +6531,7 @@
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A396">
-        <v>913983</v>
+        <v>913.98299999999995</v>
       </c>
       <c r="B396" t="s">
         <v>474</v>
@@ -6539,7 +6539,7 @@
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A397">
-        <v>916294</v>
+        <v>916.29399999999998</v>
       </c>
       <c r="B397" t="s">
         <v>475</v>
@@ -6547,7 +6547,7 @@
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A398">
-        <v>918602</v>
+        <v>918.60199999999998</v>
       </c>
       <c r="B398" t="s">
         <v>476</v>
@@ -6555,7 +6555,7 @@
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A399">
-        <v>920910</v>
+        <v>920.91</v>
       </c>
       <c r="B399" t="s">
         <v>477</v>
@@ -6566,7 +6566,7 @@
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A400">
-        <v>923215</v>
+        <v>923.21500000000003</v>
       </c>
       <c r="B400" t="s">
         <v>478</v>
@@ -6574,7 +6574,7 @@
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A401">
-        <v>925524</v>
+        <v>925.524</v>
       </c>
       <c r="B401" t="s">
         <v>479</v>
@@ -6585,7 +6585,7 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A402">
-        <v>927837</v>
+        <v>927.83699999999999</v>
       </c>
       <c r="B402" t="s">
         <v>480</v>
@@ -6596,7 +6596,7 @@
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A403">
-        <v>930132</v>
+        <v>930.13199999999995</v>
       </c>
       <c r="B403" t="s">
         <v>482</v>
@@ -6607,7 +6607,7 @@
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A404">
-        <v>932468</v>
+        <v>932.46799999999996</v>
       </c>
       <c r="B404" t="s">
         <v>483</v>
@@ -6615,7 +6615,7 @@
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A405">
-        <v>934772</v>
+        <v>934.77200000000005</v>
       </c>
       <c r="B405" t="s">
         <v>484</v>
@@ -6623,7 +6623,7 @@
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A406">
-        <v>937073</v>
+        <v>937.07299999999998</v>
       </c>
       <c r="B406" t="s">
         <v>485</v>
@@ -6634,7 +6634,7 @@
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A407">
-        <v>939403</v>
+        <v>939.40300000000002</v>
       </c>
       <c r="B407" t="s">
         <v>486</v>
@@ -6645,7 +6645,7 @@
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A408">
-        <v>941713</v>
+        <v>941.71299999999997</v>
       </c>
       <c r="B408" t="s">
         <v>487</v>
@@ -6653,7 +6653,7 @@
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A409">
-        <v>944028</v>
+        <v>944.02800000000002</v>
       </c>
       <c r="B409" t="s">
         <v>488</v>
@@ -6664,7 +6664,7 @@
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A410">
-        <v>946345</v>
+        <v>946.34500000000003</v>
       </c>
       <c r="B410" t="s">
         <v>489</v>
@@ -6672,7 +6672,7 @@
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A411">
-        <v>948399</v>
+        <v>948.399</v>
       </c>
       <c r="B411" t="s">
         <v>490</v>
@@ -6680,7 +6680,7 @@
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A412">
-        <v>950702</v>
+        <v>950.702</v>
       </c>
       <c r="B412" t="s">
         <v>491</v>
@@ -6688,7 +6688,7 @@
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A413">
-        <v>953023</v>
+        <v>953.02300000000002</v>
       </c>
       <c r="B413" t="s">
         <v>492</v>
@@ -6696,7 +6696,7 @@
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A414">
-        <v>955343</v>
+        <v>955.34299999999996</v>
       </c>
       <c r="B414" t="s">
         <v>493</v>
@@ -6704,7 +6704,7 @@
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A415">
-        <v>957672</v>
+        <v>957.67200000000003</v>
       </c>
       <c r="B415" t="s">
         <v>494</v>
@@ -6712,7 +6712,7 @@
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A416">
-        <v>959992</v>
+        <v>959.99199999999996</v>
       </c>
       <c r="B416" t="s">
         <v>495</v>
@@ -6723,7 +6723,7 @@
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A417">
-        <v>962313</v>
+        <v>962.31299999999999</v>
       </c>
       <c r="B417" t="s">
         <v>497</v>
@@ -6734,7 +6734,7 @@
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A418">
-        <v>964633</v>
+        <v>964.63300000000004</v>
       </c>
       <c r="B418" t="s">
         <v>498</v>
@@ -6745,7 +6745,7 @@
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A419">
-        <v>966923</v>
+        <v>966.923</v>
       </c>
       <c r="B419" t="s">
         <v>499</v>
@@ -6756,7 +6756,7 @@
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A420">
-        <v>968982</v>
+        <v>968.98199999999997</v>
       </c>
       <c r="B420" t="s">
         <v>500</v>
@@ -6764,7 +6764,7 @@
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A421">
-        <v>971282</v>
+        <v>971.28200000000004</v>
       </c>
       <c r="B421" t="s">
         <v>501</v>
@@ -6775,7 +6775,7 @@
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A422">
-        <v>973602</v>
+        <v>973.60199999999998</v>
       </c>
       <c r="B422" t="s">
         <v>502</v>
@@ -6783,7 +6783,7 @@
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A423">
-        <v>975922</v>
+        <v>975.92200000000003</v>
       </c>
       <c r="B423" t="s">
         <v>503</v>
@@ -6794,7 +6794,7 @@
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A424">
-        <v>978225</v>
+        <v>978.22500000000002</v>
       </c>
       <c r="B424" t="s">
         <v>504</v>
@@ -6802,7 +6802,7 @@
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A425">
-        <v>980520</v>
+        <v>980.52</v>
       </c>
       <c r="B425" t="s">
         <v>506</v>
@@ -6813,7 +6813,7 @@
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A426">
-        <v>982849</v>
+        <v>982.84900000000005</v>
       </c>
       <c r="B426" t="s">
         <v>507</v>
@@ -6824,7 +6824,7 @@
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A427">
-        <v>985162</v>
+        <v>985.16200000000003</v>
       </c>
       <c r="B427" t="s">
         <v>508</v>
@@ -6835,7 +6835,7 @@
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A428">
-        <v>987462</v>
+        <v>987.46199999999999</v>
       </c>
       <c r="B428" t="s">
         <v>509</v>
@@ -6846,7 +6846,7 @@
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A429">
-        <v>989787</v>
+        <v>989.78700000000003</v>
       </c>
       <c r="B429" t="s">
         <v>510</v>
@@ -6854,7 +6854,7 @@
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A430">
-        <v>992103</v>
+        <v>992.10299999999995</v>
       </c>
       <c r="B430" t="s">
         <v>511</v>
@@ -6865,7 +6865,7 @@
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A431">
-        <v>994424</v>
+        <v>994.42399999999998</v>
       </c>
       <c r="B431" t="s">
         <v>512</v>
@@ -6876,7 +6876,7 @@
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A432">
-        <v>996753</v>
+        <v>996.75300000000004</v>
       </c>
       <c r="B432" t="s">
         <v>513</v>
@@ -6887,7 +6887,7 @@
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A433">
-        <v>999054</v>
+        <v>999.05399999999997</v>
       </c>
       <c r="B433" t="s">
         <v>514</v>
@@ -6898,7 +6898,7 @@
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A434">
-        <v>1001342</v>
+        <v>1001.342</v>
       </c>
       <c r="B434" t="s">
         <v>2</v>
@@ -6906,7 +6906,7 @@
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A435">
-        <v>1003665</v>
+        <v>1003.665</v>
       </c>
       <c r="B435" t="s">
         <v>3</v>
@@ -6914,7 +6914,7 @@
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A436">
-        <v>1005963</v>
+        <v>1005.963</v>
       </c>
       <c r="B436" t="s">
         <v>4</v>
@@ -6925,7 +6925,7 @@
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A437">
-        <v>1008262</v>
+        <v>1008.2619999999999</v>
       </c>
       <c r="B437" t="s">
         <v>5</v>
@@ -6933,7 +6933,7 @@
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A438">
-        <v>1010561</v>
+        <v>1010.561</v>
       </c>
       <c r="B438" t="s">
         <v>6</v>
@@ -6944,7 +6944,7 @@
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A439">
-        <v>1012632</v>
+        <v>1012.6319999999999</v>
       </c>
       <c r="B439" t="s">
         <v>7</v>
@@ -6955,7 +6955,7 @@
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A440">
-        <v>1014953</v>
+        <v>1014.953</v>
       </c>
       <c r="B440" t="s">
         <v>8</v>
@@ -6966,7 +6966,7 @@
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A441">
-        <v>1017267</v>
+        <v>1017.2670000000001</v>
       </c>
       <c r="B441" t="s">
         <v>9</v>
@@ -6977,7 +6977,7 @@
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A442">
-        <v>1019563</v>
+        <v>1019.563</v>
       </c>
       <c r="B442" t="s">
         <v>10</v>
@@ -6988,7 +6988,7 @@
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A443">
-        <v>1021852</v>
+        <v>1021.852</v>
       </c>
       <c r="B443" t="s">
         <v>11</v>
@@ -6999,7 +6999,7 @@
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A444">
-        <v>1024171</v>
+        <v>1024.171</v>
       </c>
       <c r="B444" t="s">
         <v>12</v>
@@ -7010,7 +7010,7 @@
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A445">
-        <v>1026498</v>
+        <v>1026.498</v>
       </c>
       <c r="B445" t="s">
         <v>13</v>
@@ -7021,7 +7021,7 @@
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A446">
-        <v>1028802</v>
+        <v>1028.8019999999999</v>
       </c>
       <c r="B446" t="s">
         <v>14</v>
@@ -7032,7 +7032,7 @@
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A447">
-        <v>1031128</v>
+        <v>1031.1279999999999</v>
       </c>
       <c r="B447" t="s">
         <v>16</v>
@@ -7040,7 +7040,7 @@
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A448">
-        <v>1033462</v>
+        <v>1033.462</v>
       </c>
       <c r="B448" t="s">
         <v>17</v>
@@ -7048,7 +7048,7 @@
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A449">
-        <v>1035565</v>
+        <v>1035.5650000000001</v>
       </c>
       <c r="B449" t="s">
         <v>18</v>
@@ -7056,7 +7056,7 @@
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A450">
-        <v>1037891</v>
+        <v>1037.8910000000001</v>
       </c>
       <c r="B450" t="s">
         <v>19</v>
@@ -7064,7 +7064,7 @@
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A451">
-        <v>1040202</v>
+        <v>1040.202</v>
       </c>
       <c r="B451" t="s">
         <v>20</v>
@@ -7072,7 +7072,7 @@
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A452">
-        <v>1042512</v>
+        <v>1042.5119999999999</v>
       </c>
       <c r="B452" t="s">
         <v>21</v>
@@ -7080,7 +7080,7 @@
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A453">
-        <v>1044806</v>
+        <v>1044.806</v>
       </c>
       <c r="B453" t="s">
         <v>22</v>
@@ -7088,7 +7088,7 @@
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A454">
-        <v>1047110</v>
+        <v>1047.1099999999999</v>
       </c>
       <c r="B454" t="s">
         <v>23</v>
@@ -7096,7 +7096,7 @@
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A455">
-        <v>1049420</v>
+        <v>1049.42</v>
       </c>
       <c r="B455" t="s">
         <v>24</v>
@@ -7107,7 +7107,7 @@
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A456">
-        <v>1051743</v>
+        <v>1051.7429999999999</v>
       </c>
       <c r="B456" t="s">
         <v>26</v>
@@ -7118,7 +7118,7 @@
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A457">
-        <v>1054055</v>
+        <v>1054.0550000000001</v>
       </c>
       <c r="B457" t="s">
         <v>27</v>
@@ -7129,7 +7129,7 @@
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A458">
-        <v>1056350</v>
+        <v>1056.3499999999999</v>
       </c>
       <c r="B458" t="s">
         <v>28</v>
@@ -7140,7 +7140,7 @@
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A459">
-        <v>1058654</v>
+        <v>1058.654</v>
       </c>
       <c r="B459" t="s">
         <v>29</v>
@@ -7148,7 +7148,7 @@
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A460">
-        <v>1060712</v>
+        <v>1060.712</v>
       </c>
       <c r="B460" t="s">
         <v>30</v>
@@ -7156,7 +7156,7 @@
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A461">
-        <v>1063251</v>
+        <v>1063.251</v>
       </c>
       <c r="B461" t="s">
         <v>31</v>
@@ -7167,7 +7167,7 @@
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A462">
-        <v>1065307</v>
+        <v>1065.307</v>
       </c>
       <c r="B462" t="s">
         <v>32</v>
@@ -7178,7 +7178,7 @@
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A463">
-        <v>1067622</v>
+        <v>1067.6220000000001</v>
       </c>
       <c r="B463" t="s">
         <v>33</v>
@@ -7186,7 +7186,7 @@
     </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A464">
-        <v>1069940</v>
+        <v>1069.94</v>
       </c>
       <c r="B464" t="s">
         <v>34</v>
@@ -7197,7 +7197,7 @@
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A465">
-        <v>1072252</v>
+        <v>1072.252</v>
       </c>
       <c r="B465" t="s">
         <v>36</v>
@@ -7205,7 +7205,7 @@
     </row>
     <row r="466" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A466">
-        <v>1074552</v>
+        <v>1074.5519999999999</v>
       </c>
       <c r="B466" t="s">
         <v>37</v>
@@ -7216,7 +7216,7 @@
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A467">
-        <v>1076861</v>
+        <v>1076.8610000000001</v>
       </c>
       <c r="B467" t="s">
         <v>38</v>
@@ -7227,7 +7227,7 @@
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A468">
-        <v>1079254</v>
+        <v>1079.2539999999999</v>
       </c>
       <c r="B468" t="s">
         <v>39</v>
@@ -7235,7 +7235,7 @@
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A469">
-        <v>1081507</v>
+        <v>1081.5070000000001</v>
       </c>
       <c r="B469" t="s">
         <v>40</v>
@@ -7243,7 +7243,7 @@
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A470">
-        <v>1083802</v>
+        <v>1083.8019999999999</v>
       </c>
       <c r="B470" t="s">
         <v>41</v>
@@ -7254,7 +7254,7 @@
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A471">
-        <v>1086140</v>
+        <v>1086.1400000000001</v>
       </c>
       <c r="B471" t="s">
         <v>42</v>
@@ -7262,7 +7262,7 @@
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A472">
-        <v>1088458</v>
+        <v>1088.4580000000001</v>
       </c>
       <c r="B472" t="s">
         <v>43</v>
@@ -7273,7 +7273,7 @@
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A473">
-        <v>1090773</v>
+        <v>1090.7729999999999</v>
       </c>
       <c r="B473" t="s">
         <v>44</v>
@@ -7284,7 +7284,7 @@
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A474">
-        <v>1093074</v>
+        <v>1093.0740000000001</v>
       </c>
       <c r="B474" t="s">
         <v>45</v>
@@ -7292,7 +7292,7 @@
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A475">
-        <v>1095372</v>
+        <v>1095.3720000000001</v>
       </c>
       <c r="B475" t="s">
         <v>46</v>
@@ -7303,7 +7303,7 @@
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A476">
-        <v>1097442</v>
+        <v>1097.442</v>
       </c>
       <c r="B476" t="s">
         <v>47</v>
@@ -7314,7 +7314,7 @@
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A477">
-        <v>1099762</v>
+        <v>1099.7619999999999</v>
       </c>
       <c r="B477" t="s">
         <v>48</v>
@@ -7322,7 +7322,7 @@
     </row>
     <row r="478" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A478">
-        <v>1102068</v>
+        <v>1102.068</v>
       </c>
       <c r="B478" t="s">
         <v>50</v>
@@ -7333,7 +7333,7 @@
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A479">
-        <v>1104373</v>
+        <v>1104.373</v>
       </c>
       <c r="B479" t="s">
         <v>51</v>
@@ -7344,7 +7344,7 @@
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A480">
-        <v>1106690</v>
+        <v>1106.69</v>
       </c>
       <c r="B480" t="s">
         <v>52</v>
@@ -7355,7 +7355,7 @@
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A481">
-        <v>1108988</v>
+        <v>1108.9880000000001</v>
       </c>
       <c r="B481" t="s">
         <v>53</v>
@@ -7366,7 +7366,7 @@
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A482">
-        <v>1111322</v>
+        <v>1111.3219999999999</v>
       </c>
       <c r="B482" t="s">
         <v>54</v>
@@ -7374,7 +7374,7 @@
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A483">
-        <v>1113642</v>
+        <v>1113.6420000000001</v>
       </c>
       <c r="B483" t="s">
         <v>55</v>
@@ -7385,7 +7385,7 @@
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A484">
-        <v>1115963</v>
+        <v>1115.963</v>
       </c>
       <c r="B484" t="s">
         <v>56</v>
@@ -7396,7 +7396,7 @@
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A485">
-        <v>1118022</v>
+        <v>1118.0219999999999</v>
       </c>
       <c r="B485" t="s">
         <v>57</v>
@@ -7404,7 +7404,7 @@
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A486">
-        <v>1120342</v>
+        <v>1120.3420000000001</v>
       </c>
       <c r="B486" t="s">
         <v>59</v>
@@ -7412,7 +7412,7 @@
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A487">
-        <v>1122670</v>
+        <v>1122.67</v>
       </c>
       <c r="B487" t="s">
         <v>60</v>
@@ -7420,7 +7420,7 @@
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A488">
-        <v>1124972</v>
+        <v>1124.972</v>
       </c>
       <c r="B488" t="s">
         <v>61</v>
@@ -7428,7 +7428,7 @@
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A489">
-        <v>1127302</v>
+        <v>1127.3019999999999</v>
       </c>
       <c r="B489" t="s">
         <v>62</v>
@@ -7439,7 +7439,7 @@
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A490">
-        <v>1129613</v>
+        <v>1129.6130000000001</v>
       </c>
       <c r="B490" t="s">
         <v>63</v>
@@ -7450,7 +7450,7 @@
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A491">
-        <v>1131933</v>
+        <v>1131.933</v>
       </c>
       <c r="B491" t="s">
         <v>64</v>
@@ -7461,7 +7461,7 @@
     </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A492">
-        <v>1134250</v>
+        <v>1134.25</v>
       </c>
       <c r="B492" t="s">
         <v>65</v>
@@ -7472,7 +7472,7 @@
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A493">
-        <v>1136312</v>
+        <v>1136.3119999999999</v>
       </c>
       <c r="B493" t="s">
         <v>66</v>
@@ -7483,7 +7483,7 @@
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A494">
-        <v>1138642</v>
+        <v>1138.6420000000001</v>
       </c>
       <c r="B494" t="s">
         <v>67</v>
@@ -7494,7 +7494,7 @@
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A495">
-        <v>1140948</v>
+        <v>1140.9480000000001</v>
       </c>
       <c r="B495" t="s">
         <v>69</v>
@@ -7502,7 +7502,7 @@
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A496">
-        <v>1143267</v>
+        <v>1143.2670000000001</v>
       </c>
       <c r="B496" t="s">
         <v>70</v>
@@ -7510,7 +7510,7 @@
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A497">
-        <v>1145559</v>
+        <v>1145.559</v>
       </c>
       <c r="B497" t="s">
         <v>71</v>
@@ -7518,7 +7518,7 @@
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A498">
-        <v>1147873</v>
+        <v>1147.873</v>
       </c>
       <c r="B498" t="s">
         <v>72</v>
@@ -7526,7 +7526,7 @@
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A499">
-        <v>1150172</v>
+        <v>1150.172</v>
       </c>
       <c r="B499" t="s">
         <v>73</v>
@@ -7537,7 +7537,7 @@
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A500">
-        <v>1152497</v>
+        <v>1152.4970000000001</v>
       </c>
       <c r="B500" t="s">
         <v>74</v>
@@ -7545,7 +7545,7 @@
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A501">
-        <v>1154812</v>
+        <v>1154.8119999999999</v>
       </c>
       <c r="B501" t="s">
         <v>75</v>
@@ -7556,7 +7556,7 @@
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A502">
-        <v>1157122</v>
+        <v>1157.1220000000001</v>
       </c>
       <c r="B502" t="s">
         <v>76</v>
@@ -7567,7 +7567,7 @@
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A503">
-        <v>1159442</v>
+        <v>1159.442</v>
       </c>
       <c r="B503" t="s">
         <v>77</v>
@@ -7578,7 +7578,7 @@
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A504">
-        <v>1161764</v>
+        <v>1161.7639999999999</v>
       </c>
       <c r="B504" t="s">
         <v>78</v>
@@ -7589,7 +7589,7 @@
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A505">
-        <v>1164089</v>
+        <v>1164.0889999999999</v>
       </c>
       <c r="B505" t="s">
         <v>79</v>
@@ -7597,7 +7597,7 @@
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A506">
-        <v>1166152</v>
+        <v>1166.152</v>
       </c>
       <c r="B506" t="s">
         <v>80</v>
@@ -7605,7 +7605,7 @@
     </row>
     <row r="507" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A507">
-        <v>1168463</v>
+        <v>1168.463</v>
       </c>
       <c r="B507" t="s">
         <v>81</v>
@@ -7616,7 +7616,7 @@
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A508">
-        <v>1170767</v>
+        <v>1170.7670000000001</v>
       </c>
       <c r="B508" t="s">
         <v>83</v>
@@ -7627,7 +7627,7 @@
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A509">
-        <v>1173095</v>
+        <v>1173.095</v>
       </c>
       <c r="B509" t="s">
         <v>84</v>
@@ -7638,7 +7638,7 @@
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A510">
-        <v>1175436</v>
+        <v>1175.4359999999999</v>
       </c>
       <c r="B510" t="s">
         <v>85</v>
@@ -7646,7 +7646,7 @@
     </row>
     <row r="511" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A511">
-        <v>1177722</v>
+        <v>1177.722</v>
       </c>
       <c r="B511" t="s">
         <v>86</v>
@@ -7657,7 +7657,7 @@
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A512">
-        <v>1180032</v>
+        <v>1180.0319999999999</v>
       </c>
       <c r="B512" t="s">
         <v>87</v>
@@ -7668,7 +7668,7 @@
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A513">
-        <v>1182362</v>
+        <v>1182.3620000000001</v>
       </c>
       <c r="B513" t="s">
         <v>88</v>
@@ -7679,7 +7679,7 @@
     </row>
     <row r="514" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A514">
-        <v>1184677</v>
+        <v>1184.6769999999999</v>
       </c>
       <c r="B514" t="s">
         <v>89</v>
@@ -7687,7 +7687,7 @@
     </row>
     <row r="515" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A515">
-        <v>1186967</v>
+        <v>1186.9670000000001</v>
       </c>
       <c r="B515" t="s">
         <v>90</v>
@@ -7698,7 +7698,7 @@
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A516">
-        <v>1190020</v>
+        <v>1190.02</v>
       </c>
       <c r="B516" t="s">
         <v>92</v>
@@ -7708,9 +7708,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C516" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C516">
-      <sortCondition ref="A1:A516"/>
+  <autoFilter ref="A1:D517" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D517">
+      <sortCondition ref="A1:A517"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
crop width and filters applied
</commit_message>
<xml_diff>
--- a/Screenshots/pilot_ep_1.xlsx
+++ b/Screenshots/pilot_ep_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\linux\scratches\Netflix_image_subtitle_crawler\Screenshots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457C49D4-6287-46C5-9F64-BD97EDA79F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76902CA3-29EF-4EE8-86C8-E0E2E9F6CEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6230" yWindow="-200" windowWidth="12000" windowHeight="6170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6700" yWindow="-50" windowWidth="14400" windowHeight="7030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="783">
   <si>
     <t>time(sec)</t>
   </si>
@@ -1588,7 +1588,7 @@
     <t>छोड़ो भी, मैं तुम्हें हल्का करने की कोशिश कर रहा हूँ।</t>
   </si>
   <si>
-    <t>मुझे हल्का होने की ज़रूरत नहीं। मेरी दुनिया में अंधेरा है।</t>
+    <t>मुझे हल्का होने की ज़रूरत नहीं मेरी दुनिया में अंधेरा है।</t>
   </si>
   <si>
     <t>अंधेरा और बरसाती।</t>
@@ -1603,18 +1603,12 @@
     <t>बेशक, वह एक गलती थी।</t>
   </si>
   <si>
-    <t>तुम्हें पूरा यकीन है?</t>
-  </si>
-  <si>
     <t>शायद हमें एक सूची बनानी चाहिए।</t>
   </si>
   <si>
     <t>क्या हो रहा है? नींद नहीं आई?</t>
   </si>
   <si>
-    <t>नहीं।</t>
-  </si>
-  <si>
     <t>मेरे डैड ने कहा हम कल दादी माँ के घर जा रहे हैं।</t>
   </si>
   <si>
@@ -1645,7 +1639,7 @@
     <t>शायद मैं इस दुनिया में सबसे अधिक खुद से प्यार करता हूँ।</t>
   </si>
   <si>
-    <t>चार्ली? जल,</t>
+    <t>चार्ली?</t>
   </si>
   <si>
     <t>मुझे दादी माँ के घर नहीं जाना। यहाँ रहना है।</t>
@@ -1660,7 +1654,7 @@
     <t>ठीक है।</t>
   </si>
   <si>
-    <t>यह रुकेगी? क्योंकि मैंने अपनी कार इसकी कार के पीछे लगाई है।</t>
+    <t>यह रुकेगी? क्‍योंकि मैंने अपनी कार इसकी कार के पीछे लगाई है।</t>
   </si>
   <si>
     <t>उस जैसे बच्चे से प्यार हो जाता है।</t>
@@ -1681,7 +1675,7 @@
     <t>तुम्हें अपने भतीजे के बारे में बात करनी है, या सेक्स करना है?</t>
   </si>
   <si>
-    <t>है: कुछ पूछना ही त्ि</t>
+    <t>कुछ हर है।</t>
   </si>
   <si>
     <t>वाह, हमारी बढ़िया जम रही है। क्या हम इसी तक रहने दें?</t>
@@ -1690,10 +1684,10 @@
     <t>तुम क्या कर रही हो? मुझे लगा हम सेक्स करने वाले थे।</t>
   </si>
   <si>
-    <t>मैं कैसे सेक्स करूँ: जबकि तुम बच्चे पैदा करने के बारे में सोच रहे हो?</t>
-  </si>
-  <si>
-    <t>नलिउ। कि है: है 4है+॥| बीप की आवाज़ सुनते ही अपनी बात कहें।</t>
+    <t>मैं कैसे सेक्‍स करूँ जबकि तुम बच्चे पैदा करने के बारे में सोच रहे हो?</t>
+  </si>
+  <si>
+    <t>हेलो, चार्ली बोल रहा हूँ। बीप की आवाज़ सुनते ही अपनी बात कहें।</t>
   </si>
   <si>
     <t>हेलो, मंकी मैन।</t>
@@ -1702,7 +1696,7 @@
     <t>मैं तुम्हारे बारे में सोच रही थी,</t>
   </si>
   <si>
-    <t>और जानना था कि हम एक-दूसरे को इतना दुख क्यों देते हैं।</t>
+    <t>और जानना था कि हम एक-दूसरे को इतना दुख क्‍यों देते हैं।</t>
   </si>
   <si>
     <t>रोज़, मैं बोल रहा हूँ, मंकी मैन।</t>
@@ -1714,7 +1708,7 @@
     <t>किसी औरत से यह पूछना स्वाभाविक तौर पर गलत है</t>
   </si>
   <si>
-    <t>0०५ ॥।।। ०१० यह हम दोनों के लिए है। जाना मत।</t>
+    <t>यह हम दोनों के लिए है। जाना मत।</t>
   </si>
   <si>
     <t>बारह साल, और उसने मुझे निकाल दिया।</t>
@@ -1735,13 +1729,13 @@
     <t>कि तुम्हारे पायदान पर हो।</t>
   </si>
   <si>
-    <t>माफ़ करना, पर अगर तुम नकली पत्थर को दूसरे पत्थरों के ढेर में रखोगे,</t>
+    <t>माफ़ करना, पर अगर तुम नकली पत्थर को दूसरे पत्थरों के ढेर में रखोगे</t>
   </si>
   <si>
     <t>तो नशे की हालत में उसे ढूँढना कठिन होगा।</t>
   </si>
   <si>
-    <t>चिंता मत करो। मेरे पैरों में इतना खून नहीं बचा कि कहीं और जा सकूँ।</t>
+    <t>चिंता मत करो। मेरे पैरों में इतना खून नहीं बचा कि कहीं और जा सकू।</t>
   </si>
   <si>
     <t>मैं एक अच्छा पति हूँ। भरोसेमंद हूँ।</t>
@@ -1792,7 +1786,7 @@
     <t>अधिक से अधिक कुछ दिन। उसका दिमाग ठिकाने जाएगा।</t>
   </si>
   <si>
-    <t>हाँ। औरतें यही करती हैं।</t>
+    <t>हा। औरतें यही करती हैं।</t>
   </si>
   <si>
     <t>मेहमान वाले कमरे में रहो। मैं चादरें लाता हूँ।</t>
@@ -1804,7 +1798,7 @@
     <t>मुझे अपनी चादरें पसंद हैं।</t>
   </si>
   <si>
-    <t>है, फ़िर, गुड नाइट। का</t>
+    <t>है, फ़िर, गुड नाइट। रुको।</t>
   </si>
   <si>
     <t>हम मुश्किल से एक-दूसरे से बात करते हैं।</t>
@@ -1819,9 +1813,6 @@
     <t>मुझे काइरोप्रैक्टर ऑफ़ ईयर नामित किया।</t>
   </si>
   <si>
-    <t>हेलो, चार्ली बोल रहा हूँ। बीप की आवाज़ सुनते ही अपनी बात कहें।</t>
-  </si>
-  <si>
     <t>है, फ़िर। गुड नाइट।</t>
   </si>
   <si>
@@ -1849,7 +1840,7 @@
     <t>है। गुड नाइट, चार्ली। नाइट।</t>
   </si>
   <si>
-    <t>सुनो, घटिया इंसान, मैं अपने साथ ऐसा बर्ताव नहीं होने दूँगी।</t>
+    <t>सुनो, घटिया इंसान, मैं अपने साथ ऐसा बर्ताव नहीं होने टूँगी।</t>
   </si>
   <si>
     <t>अरे, आपकी आँखें लाल हैं।</t>
@@ -1858,9 +1849,6 @@
     <t>मेरी आँखों से देखना चाहिए।</t>
   </si>
   <si>
-    <t>आर ८ट95आ0०98९80: ०१: ५०१३ की</t>
-  </si>
-  <si>
     <t>मेरी माँ मुझे लाईं।</t>
   </si>
   <si>
@@ -1909,10 +1897,10 @@
     <t>ठीक है, तो यह शायद की ओर रहेगा।</t>
   </si>
   <si>
-    <t>मैं झूठ क्यों बोलूँगा? आज समुद्र बंद है।</t>
-  </si>
-  <si>
-    <t>हे राम, तुम्हें नहीं लगता कि तुम पैंट पहन लो?</t>
+    <t>मैं झूठ क्यों बोलँगा? आज समुद्र बंद है।</t>
+  </si>
+  <si>
+    <t>है राम, तुम्हें नहीं लगता कि तुम पैंट पहन लो?</t>
   </si>
   <si>
     <t>मुझे देखो, जूडी। मुझे पैंट पहनने का समय नहीं मिला।</t>
@@ -1939,7 +1927,7 @@
     <t>वह कौन थी?</t>
   </si>
   <si>
-    <t>मेरे माँ-बाप अलग हो रहे हैं।</t>
+    <t>मेरे मॉा-बाप अलग हो रहे हैं।</t>
   </si>
   <si>
     <t>हाँ। यह ऐसा लगता तो है।</t>
@@ -1981,9 +1969,6 @@
     <t>इसके लिए लंच बना दोगे?</t>
   </si>
   <si>
-    <t>१॥72॥॥</t>
-  </si>
-  <si>
     <t>तुम क्यों मुस्करा रहे हो?</t>
   </si>
   <si>
@@ -2017,7 +2002,7 @@
     <t>अच्छा, यह एक औरत है जिसके साथ एक बार बाहर गया और वह थोड़ी चिपकू हो गई।</t>
   </si>
   <si>
-    <t>होशियार हो। लगे रहो। तुम उनमें से एक कार्टन पर होगे।</t>
+    <t>होशियार होौ। लगे रहो। तुम उनमें से एक कार्टन पर होगे।</t>
   </si>
   <si>
     <t>ठीक है, कॉर्नफ्लेक्स।</t>
@@ -2041,7 +2026,7 @@
     <t>चार्ली ने लिखा। नहीं?</t>
   </si>
   <si>
-    <t>अगर झूठ बोलना होता तो कहता स्टेयरवे टू हेवन लिखा,</t>
+    <t>अगर झूठ बोलना होता तो कहता स्टेयरवे ट्‌ हेवन लिखा,</t>
   </si>
   <si>
     <t>लोगों की खूब बनती है।</t>
@@ -2056,19 +2041,19 @@
     <t>डॉ. ब्लूम? हाँ, एलन हार्पर बोल रहा हूँ।</t>
   </si>
   <si>
-    <t>मेरी पत्नी मैं दोपहर की हमारी शादी के परामर्श की अपॉइंटमेंट रह्द करना चाहते हैं।</t>
+    <t>मेरी पत्नी मैं दोपहर की हमारी शादी के परामर्श की अपॉइंटमेंट रद्द करना चाहते हैं।</t>
   </si>
   <si>
     <t>हाँ, ख़ैर, कुछ काम गया।</t>
   </si>
   <si>
-    <t>ख़ैर, यह थोड़ा निजी है। मेरा मतलब</t>
+    <t>ख़ेर, यह थोडा निजी है। मेरा मतलब</t>
   </si>
   <si>
     <t>और फिर भी, तमाचे हमेशा तुम्हें पड़ते हैं।</t>
   </si>
   <si>
-    <t>हाँ, इन बातों की अहमियत जानता हूँ.</t>
+    <t>हाँ, इन बातों की अहमियत जानता हूँ--</t>
   </si>
   <si>
     <t>चार्ली घर पर है?</t>
@@ -2116,7 +2101,7 @@
     <t>हेलो, चार्ली बोल रहा हूँ। बीप की आवाज़ पर अपनी बात कहें।</t>
   </si>
   <si>
-    <t>यह क्‍यों मान रहे हो</t>
+    <t>यह क्‍यों मान रहे हो कि उसने मुझसे सीखा?</t>
   </si>
   <si>
     <t>के लिए शुक्रिया। मैंने नहीं की। रोज़ आई थी।</t>
@@ -2176,7 +2161,7 @@
     <t>कोई ख़ास बात नहीं, बस बात करना चाहता था।</t>
   </si>
   <si>
-    <t>आप मेरे घर में कैसे आईं?</t>
+    <t>आप मेरे घर में कैसे आई?</t>
   </si>
   <si>
     <t>मैं तुम्हारे भाई के मुश्किल समय में मदद के लिए आई।</t>
@@ -2212,7 +2197,7 @@
     <t>आइस्ड टी, दादी माँ। नन्हे फ़रिश्ते।</t>
   </si>
   <si>
-    <t>जानू, नीबू की फाँक माँगी थी।</t>
+    <t>जानू, नीबू की फाॉँक माँगी थी।</t>
   </si>
   <si>
     <t>अच्छा। अब सुनो तुम क्या करोगे।</t>
@@ -2230,7 +2215,7 @@
     <t>मैं अपने घर वापस चला जाऊँगा।</t>
   </si>
   <si>
-    <t>जान, बड़े हो जाओ।</t>
+    <t>जान, बडे हो जाओ।</t>
   </si>
   <si>
     <t>जो कहा उसके बारे में सोचो।</t>
@@ -2293,7 +2278,7 @@
     <t>मैं भी।</t>
   </si>
   <si>
-    <t>मैं एक डॉलर डालता हूँ और पाँच डॉलर की चाल चलता हूँ।</t>
+    <t>में एक डॉलर डालता हूँ और पाँच डॉलर की चाल चलता हूँ।</t>
   </si>
   <si>
     <t>देखना चाहूँगा। भी।</t>
@@ -2329,7 +2314,7 @@
     <t>ख़ैर, हाँ, मुझे लगता है कि तुम यहाँ रह सकते हो।</t>
   </si>
   <si>
-    <t>और डॉलर की चाल चलूँगा।</t>
+    <t>और डॉलर की चाल चलूगा।</t>
   </si>
   <si>
     <t>लगता है उसने फँसा लिया। झाँसा दे रहा है।</t>
@@ -2377,7 +2362,7 @@
     <t>तो, डिनर कैसा था?</t>
   </si>
   <si>
-    <t>कुछ घंटों के लिए तुम्हें उसके साथ अकेले छोड़ता हूँ.</t>
+    <t>कुछ घंटों के लिए तुम्हें उसके साथ अकेले छोड़ता हूँ--</t>
   </si>
   <si>
     <t>डिनर बढ़िया था। हमने वील पिकाटा खाई और वह समलैंगिक है!</t>
@@ -2764,13 +2749,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C516"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79:XFD79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="67" bestFit="1" customWidth="1"/>
   </cols>
@@ -2793,9 +2778,6 @@
       <c r="B2" t="s">
         <v>179</v>
       </c>
-      <c r="C2" t="s">
-        <v>611</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -2805,7 +2787,7 @@
         <v>275</v>
       </c>
       <c r="C3" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -2824,7 +2806,7 @@
         <v>516</v>
       </c>
       <c r="C5" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2835,7 +2817,7 @@
         <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -2846,7 +2828,7 @@
         <v>107</v>
       </c>
       <c r="C7" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -2857,7 +2839,7 @@
         <v>117</v>
       </c>
       <c r="C8" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2884,7 +2866,7 @@
         <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>598</v>
+        <v>554</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -2903,7 +2885,7 @@
         <v>174</v>
       </c>
       <c r="C13" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -2914,7 +2896,7 @@
         <v>184</v>
       </c>
       <c r="C14" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -2925,7 +2907,7 @@
         <v>194</v>
       </c>
       <c r="C15" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -2952,7 +2934,7 @@
         <v>227</v>
       </c>
       <c r="C18" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -2971,7 +2953,7 @@
         <v>250</v>
       </c>
       <c r="C20" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -2982,7 +2964,7 @@
         <v>260</v>
       </c>
       <c r="C21" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -3001,7 +2983,7 @@
         <v>285</v>
       </c>
       <c r="C23" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -3012,7 +2994,7 @@
         <v>294</v>
       </c>
       <c r="C24" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -3023,7 +3005,7 @@
         <v>304</v>
       </c>
       <c r="C25" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -3034,7 +3016,7 @@
         <v>318</v>
       </c>
       <c r="C26" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -3069,7 +3051,7 @@
         <v>361</v>
       </c>
       <c r="C30" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -3088,7 +3070,7 @@
         <v>384</v>
       </c>
       <c r="C32" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -3099,7 +3081,7 @@
         <v>394</v>
       </c>
       <c r="C33" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -3110,7 +3092,7 @@
         <v>404</v>
       </c>
       <c r="C34" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -3121,7 +3103,7 @@
         <v>413</v>
       </c>
       <c r="C35" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -3132,7 +3114,7 @@
         <v>428</v>
       </c>
       <c r="C36" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -3143,7 +3125,7 @@
         <v>438</v>
       </c>
       <c r="C37" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -3154,7 +3136,7 @@
         <v>448</v>
       </c>
       <c r="C38" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -3181,7 +3163,7 @@
         <v>481</v>
       </c>
       <c r="C41" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -3200,7 +3182,7 @@
         <v>505</v>
       </c>
       <c r="C43" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -3211,7 +3193,7 @@
         <v>515</v>
       </c>
       <c r="C44" t="s">
-        <v>786</v>
+        <v>781</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -3254,7 +3236,7 @@
         <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -3289,7 +3271,7 @@
         <v>94</v>
       </c>
       <c r="C53" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -3300,7 +3282,7 @@
         <v>95</v>
       </c>
       <c r="C54" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -3311,7 +3293,7 @@
         <v>96</v>
       </c>
       <c r="C55" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -3322,7 +3304,7 @@
         <v>97</v>
       </c>
       <c r="C56" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -3333,7 +3315,7 @@
         <v>98</v>
       </c>
       <c r="C57" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -3352,7 +3334,7 @@
         <v>100</v>
       </c>
       <c r="C59" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -3371,7 +3353,7 @@
         <v>102</v>
       </c>
       <c r="C61" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -3382,7 +3364,7 @@
         <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -3393,7 +3375,7 @@
         <v>104</v>
       </c>
       <c r="C63" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -3404,7 +3386,7 @@
         <v>105</v>
       </c>
       <c r="C64" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -3423,7 +3405,7 @@
         <v>108</v>
       </c>
       <c r="C66" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -3450,7 +3432,7 @@
         <v>111</v>
       </c>
       <c r="C69" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -3461,7 +3443,7 @@
         <v>112</v>
       </c>
       <c r="C70" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -3472,7 +3454,7 @@
         <v>113</v>
       </c>
       <c r="C71" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -3483,7 +3465,7 @@
         <v>114</v>
       </c>
       <c r="C72" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -3494,7 +3476,7 @@
         <v>115</v>
       </c>
       <c r="C73" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -3505,7 +3487,7 @@
         <v>116</v>
       </c>
       <c r="C74" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -3524,7 +3506,7 @@
         <v>119</v>
       </c>
       <c r="C76" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -3543,7 +3525,7 @@
         <v>121</v>
       </c>
       <c r="C78" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -3554,7 +3536,7 @@
         <v>122</v>
       </c>
       <c r="C79" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -3573,7 +3555,7 @@
         <v>124</v>
       </c>
       <c r="C81" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -3592,7 +3574,7 @@
         <v>127</v>
       </c>
       <c r="C83" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -3603,7 +3585,7 @@
         <v>128</v>
       </c>
       <c r="C84" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -3614,7 +3596,7 @@
         <v>129</v>
       </c>
       <c r="C85" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -3625,7 +3607,7 @@
         <v>130</v>
       </c>
       <c r="C86" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -3644,7 +3626,7 @@
         <v>132</v>
       </c>
       <c r="C88" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -3655,7 +3637,7 @@
         <v>133</v>
       </c>
       <c r="C89" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -3666,7 +3648,7 @@
         <v>134</v>
       </c>
       <c r="C90" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -3677,7 +3659,7 @@
         <v>135</v>
       </c>
       <c r="C91" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -3696,7 +3678,7 @@
         <v>137</v>
       </c>
       <c r="C93" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -3707,7 +3689,7 @@
         <v>138</v>
       </c>
       <c r="C94" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -3726,7 +3708,7 @@
         <v>141</v>
       </c>
       <c r="C96" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -3745,7 +3727,7 @@
         <v>143</v>
       </c>
       <c r="C98" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -3756,7 +3738,7 @@
         <v>144</v>
       </c>
       <c r="C99" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -3775,7 +3757,7 @@
         <v>146</v>
       </c>
       <c r="C101" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -3786,7 +3768,7 @@
         <v>147</v>
       </c>
       <c r="C102" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -3797,7 +3779,7 @@
         <v>148</v>
       </c>
       <c r="C103" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
@@ -3808,7 +3790,7 @@
         <v>149</v>
       </c>
       <c r="C104" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -3819,7 +3801,7 @@
         <v>151</v>
       </c>
       <c r="C105" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
@@ -3830,7 +3812,7 @@
         <v>152</v>
       </c>
       <c r="C106" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
@@ -3849,7 +3831,7 @@
         <v>154</v>
       </c>
       <c r="C108" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
@@ -3860,7 +3842,7 @@
         <v>155</v>
       </c>
       <c r="C109" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -3879,7 +3861,7 @@
         <v>157</v>
       </c>
       <c r="C111" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -3890,7 +3872,7 @@
         <v>158</v>
       </c>
       <c r="C112" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
@@ -3901,7 +3883,7 @@
         <v>159</v>
       </c>
       <c r="C113" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
@@ -3912,7 +3894,7 @@
         <v>161</v>
       </c>
       <c r="C114" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
@@ -3955,7 +3937,7 @@
         <v>166</v>
       </c>
       <c r="C119" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
@@ -4022,7 +4004,7 @@
         <v>175</v>
       </c>
       <c r="C127" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
@@ -4041,7 +4023,7 @@
         <v>177</v>
       </c>
       <c r="C129" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
@@ -4060,7 +4042,7 @@
         <v>180</v>
       </c>
       <c r="C131" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
@@ -4071,7 +4053,7 @@
         <v>181</v>
       </c>
       <c r="C132" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
@@ -4090,7 +4072,7 @@
         <v>183</v>
       </c>
       <c r="C134" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
@@ -4117,7 +4099,7 @@
         <v>187</v>
       </c>
       <c r="C137" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
@@ -4128,7 +4110,7 @@
         <v>188</v>
       </c>
       <c r="C138" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
@@ -4139,7 +4121,7 @@
         <v>189</v>
       </c>
       <c r="C139" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
@@ -4150,7 +4132,7 @@
         <v>190</v>
       </c>
       <c r="C140" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
@@ -4169,7 +4151,7 @@
         <v>192</v>
       </c>
       <c r="C142" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
@@ -4188,7 +4170,7 @@
         <v>195</v>
       </c>
       <c r="C144" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
@@ -4199,7 +4181,7 @@
         <v>196</v>
       </c>
       <c r="C145" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
@@ -4210,7 +4192,7 @@
         <v>197</v>
       </c>
       <c r="C146" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
@@ -4221,7 +4203,7 @@
         <v>198</v>
       </c>
       <c r="C147" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
@@ -4232,7 +4214,7 @@
         <v>199</v>
       </c>
       <c r="C148" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
@@ -4243,7 +4225,7 @@
         <v>200</v>
       </c>
       <c r="C149" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
@@ -4254,7 +4236,7 @@
         <v>201</v>
       </c>
       <c r="C150" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
@@ -4265,7 +4247,7 @@
         <v>202</v>
       </c>
       <c r="C151" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
@@ -4284,7 +4266,7 @@
         <v>204</v>
       </c>
       <c r="C153" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
@@ -4295,7 +4277,7 @@
         <v>205</v>
       </c>
       <c r="C154" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
@@ -4306,7 +4288,7 @@
         <v>206</v>
       </c>
       <c r="C155" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
@@ -4317,7 +4299,7 @@
         <v>207</v>
       </c>
       <c r="C156" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
@@ -4336,7 +4318,7 @@
         <v>210</v>
       </c>
       <c r="C158" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
@@ -4355,7 +4337,7 @@
         <v>212</v>
       </c>
       <c r="C160" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
@@ -4366,7 +4348,7 @@
         <v>213</v>
       </c>
       <c r="C161" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
@@ -4377,7 +4359,7 @@
         <v>214</v>
       </c>
       <c r="C162" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
@@ -4412,7 +4394,7 @@
         <v>219</v>
       </c>
       <c r="C166" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
@@ -4423,7 +4405,7 @@
         <v>220</v>
       </c>
       <c r="C167" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
@@ -4434,7 +4416,7 @@
         <v>221</v>
       </c>
       <c r="C168" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
@@ -4445,7 +4427,7 @@
         <v>222</v>
       </c>
       <c r="C169" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
@@ -4472,7 +4454,7 @@
         <v>225</v>
       </c>
       <c r="C172" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
@@ -4523,7 +4505,7 @@
         <v>232</v>
       </c>
       <c r="C178" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
@@ -4534,7 +4516,7 @@
         <v>233</v>
       </c>
       <c r="C179" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
@@ -4561,7 +4543,7 @@
         <v>236</v>
       </c>
       <c r="C182" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
@@ -4588,7 +4570,7 @@
         <v>240</v>
       </c>
       <c r="C185" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
@@ -4607,7 +4589,7 @@
         <v>242</v>
       </c>
       <c r="C187" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
@@ -4634,7 +4616,7 @@
         <v>245</v>
       </c>
       <c r="C190" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
@@ -4661,7 +4643,7 @@
         <v>248</v>
       </c>
       <c r="C193" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
@@ -4680,7 +4662,7 @@
         <v>251</v>
       </c>
       <c r="C195" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
@@ -4691,7 +4673,7 @@
         <v>252</v>
       </c>
       <c r="C196" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
@@ -4726,7 +4708,7 @@
         <v>256</v>
       </c>
       <c r="C200" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
@@ -4769,7 +4751,7 @@
         <v>262</v>
       </c>
       <c r="C205" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.35">
@@ -4780,7 +4762,7 @@
         <v>263</v>
       </c>
       <c r="C206" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.35">
@@ -4798,9 +4780,6 @@
       <c r="B208" t="s">
         <v>265</v>
       </c>
-      <c r="C208" t="s">
-        <v>652</v>
-      </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A209">
@@ -4818,7 +4797,7 @@
         <v>267</v>
       </c>
       <c r="C210" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.35">
@@ -4829,7 +4808,7 @@
         <v>268</v>
       </c>
       <c r="C211" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.35">
@@ -4840,7 +4819,7 @@
         <v>269</v>
       </c>
       <c r="C212" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.35">
@@ -4859,7 +4838,7 @@
         <v>272</v>
       </c>
       <c r="C214" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.35">
@@ -4878,7 +4857,7 @@
         <v>274</v>
       </c>
       <c r="C216" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.35">
@@ -4897,7 +4876,7 @@
         <v>277</v>
       </c>
       <c r="C218" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.35">
@@ -4916,7 +4895,7 @@
         <v>279</v>
       </c>
       <c r="C220" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.35">
@@ -4927,7 +4906,7 @@
         <v>280</v>
       </c>
       <c r="C221" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.35">
@@ -4946,7 +4925,7 @@
         <v>282</v>
       </c>
       <c r="C223" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.35">
@@ -4965,7 +4944,7 @@
         <v>284</v>
       </c>
       <c r="C225" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.35">
@@ -4984,7 +4963,7 @@
         <v>287</v>
       </c>
       <c r="C227" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.35">
@@ -5011,7 +4990,7 @@
         <v>290</v>
       </c>
       <c r="C230" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.35">
@@ -5022,7 +5001,7 @@
         <v>291</v>
       </c>
       <c r="C231" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.35">
@@ -5033,7 +5012,7 @@
         <v>292</v>
       </c>
       <c r="C232" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.35">
@@ -5044,7 +5023,7 @@
         <v>293</v>
       </c>
       <c r="C233" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.35">
@@ -5055,7 +5034,7 @@
         <v>295</v>
       </c>
       <c r="C234" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.35">
@@ -5066,7 +5045,7 @@
         <v>296</v>
       </c>
       <c r="C235" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.35">
@@ -5085,7 +5064,7 @@
         <v>298</v>
       </c>
       <c r="C237" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.35">
@@ -5096,7 +5075,7 @@
         <v>299</v>
       </c>
       <c r="C238" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.35">
@@ -5107,7 +5086,7 @@
         <v>300</v>
       </c>
       <c r="C239" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.35">
@@ -5126,7 +5105,7 @@
         <v>302</v>
       </c>
       <c r="C241" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.35">
@@ -5153,7 +5132,7 @@
         <v>306</v>
       </c>
       <c r="C244" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.35">
@@ -5204,7 +5183,7 @@
         <v>312</v>
       </c>
       <c r="C250" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.35">
@@ -5215,7 +5194,7 @@
         <v>313</v>
       </c>
       <c r="C251" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.35">
@@ -5226,7 +5205,7 @@
         <v>314</v>
       </c>
       <c r="C252" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.35">
@@ -5245,7 +5224,7 @@
         <v>316</v>
       </c>
       <c r="C254" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.35">
@@ -5256,7 +5235,7 @@
         <v>317</v>
       </c>
       <c r="C255" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.35">
@@ -5275,7 +5254,7 @@
         <v>320</v>
       </c>
       <c r="C257" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.35">
@@ -5302,7 +5281,7 @@
         <v>323</v>
       </c>
       <c r="C260" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.35">
@@ -5313,7 +5292,7 @@
         <v>324</v>
       </c>
       <c r="C261" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.35">
@@ -5324,7 +5303,7 @@
         <v>325</v>
       </c>
       <c r="C262" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.35">
@@ -5335,7 +5314,7 @@
         <v>326</v>
       </c>
       <c r="C263" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.35">
@@ -5362,7 +5341,7 @@
         <v>330</v>
       </c>
       <c r="C266" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.35">
@@ -5373,7 +5352,7 @@
         <v>331</v>
       </c>
       <c r="C267" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.35">
@@ -5384,7 +5363,7 @@
         <v>332</v>
       </c>
       <c r="C268" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.35">
@@ -5451,7 +5430,7 @@
         <v>341</v>
       </c>
       <c r="C276" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.35">
@@ -5462,7 +5441,7 @@
         <v>342</v>
       </c>
       <c r="C277" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.35">
@@ -5497,7 +5476,7 @@
         <v>346</v>
       </c>
       <c r="C281" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.35">
@@ -5508,7 +5487,7 @@
         <v>347</v>
       </c>
       <c r="C282" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.35">
@@ -5551,7 +5530,7 @@
         <v>353</v>
       </c>
       <c r="C287" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.35">
@@ -5562,7 +5541,7 @@
         <v>354</v>
       </c>
       <c r="C288" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.35">
@@ -5581,7 +5560,7 @@
         <v>356</v>
       </c>
       <c r="C290" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.35">
@@ -5592,7 +5571,7 @@
         <v>357</v>
       </c>
       <c r="C291" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.35">
@@ -5611,7 +5590,7 @@
         <v>359</v>
       </c>
       <c r="C293" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.35">
@@ -5630,7 +5609,7 @@
         <v>362</v>
       </c>
       <c r="C295" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.35">
@@ -5665,7 +5644,7 @@
         <v>366</v>
       </c>
       <c r="C299" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.35">
@@ -5676,7 +5655,7 @@
         <v>367</v>
       </c>
       <c r="C300" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.35">
@@ -5687,7 +5666,7 @@
         <v>368</v>
       </c>
       <c r="C301" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.35">
@@ -5706,7 +5685,7 @@
         <v>371</v>
       </c>
       <c r="C303" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.35">
@@ -5717,7 +5696,7 @@
         <v>372</v>
       </c>
       <c r="C304" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.35">
@@ -5728,7 +5707,7 @@
         <v>373</v>
       </c>
       <c r="C305" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.35">
@@ -5739,7 +5718,7 @@
         <v>374</v>
       </c>
       <c r="C306" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.35">
@@ -5750,7 +5729,7 @@
         <v>375</v>
       </c>
       <c r="C307" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.35">
@@ -5769,7 +5748,7 @@
         <v>377</v>
       </c>
       <c r="C309" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.35">
@@ -5780,7 +5759,7 @@
         <v>378</v>
       </c>
       <c r="C310" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.35">
@@ -5791,7 +5770,7 @@
         <v>379</v>
       </c>
       <c r="C311" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.35">
@@ -5802,7 +5781,7 @@
         <v>380</v>
       </c>
       <c r="C312" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.35">
@@ -5813,7 +5792,7 @@
         <v>381</v>
       </c>
       <c r="C313" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.35">
@@ -5824,7 +5803,7 @@
         <v>382</v>
       </c>
       <c r="C314" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.35">
@@ -5835,7 +5814,7 @@
         <v>383</v>
       </c>
       <c r="C315" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.35">
@@ -5846,7 +5825,7 @@
         <v>385</v>
       </c>
       <c r="C316" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.35">
@@ -5889,7 +5868,7 @@
         <v>390</v>
       </c>
       <c r="C321" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.35">
@@ -5900,7 +5879,7 @@
         <v>391</v>
       </c>
       <c r="C322" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.35">
@@ -5911,7 +5890,7 @@
         <v>392</v>
       </c>
       <c r="C323" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.35">
@@ -5930,7 +5909,7 @@
         <v>395</v>
       </c>
       <c r="C325" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.35">
@@ -5949,7 +5928,7 @@
         <v>397</v>
       </c>
       <c r="C327" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.35">
@@ -5960,7 +5939,7 @@
         <v>398</v>
       </c>
       <c r="C328" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.35">
@@ -5971,7 +5950,7 @@
         <v>399</v>
       </c>
       <c r="C329" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.35">
@@ -5982,7 +5961,7 @@
         <v>400</v>
       </c>
       <c r="C330" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.35">
@@ -5993,7 +5972,7 @@
         <v>401</v>
       </c>
       <c r="C331" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.35">
@@ -6004,7 +5983,7 @@
         <v>402</v>
       </c>
       <c r="C332" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.35">
@@ -6015,7 +5994,7 @@
         <v>403</v>
       </c>
       <c r="C333" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.35">
@@ -6026,7 +6005,7 @@
         <v>405</v>
       </c>
       <c r="C334" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.35">
@@ -6037,7 +6016,7 @@
         <v>406</v>
       </c>
       <c r="C335" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.35">
@@ -6064,7 +6043,7 @@
         <v>409</v>
       </c>
       <c r="C338" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.35">
@@ -6075,7 +6054,7 @@
         <v>410</v>
       </c>
       <c r="C339" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.35">
@@ -6086,7 +6065,7 @@
         <v>411</v>
       </c>
       <c r="C340" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.35">
@@ -6113,7 +6092,7 @@
         <v>415</v>
       </c>
       <c r="C343" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.35">
@@ -6124,7 +6103,7 @@
         <v>416</v>
       </c>
       <c r="C344" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.35">
@@ -6135,7 +6114,7 @@
         <v>417</v>
       </c>
       <c r="C345" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.35">
@@ -6146,7 +6125,7 @@
         <v>418</v>
       </c>
       <c r="C346" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.35">
@@ -6157,7 +6136,7 @@
         <v>420</v>
       </c>
       <c r="C347" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.35">
@@ -6168,7 +6147,7 @@
         <v>421</v>
       </c>
       <c r="C348" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.35">
@@ -6179,7 +6158,7 @@
         <v>422</v>
       </c>
       <c r="C349" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.35">
@@ -6198,7 +6177,7 @@
         <v>424</v>
       </c>
       <c r="C351" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.35">
@@ -6209,7 +6188,7 @@
         <v>425</v>
       </c>
       <c r="C352" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.35">
@@ -6220,7 +6199,7 @@
         <v>426</v>
       </c>
       <c r="C353" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.35">
@@ -6279,7 +6258,7 @@
         <v>434</v>
       </c>
       <c r="C360" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.35">
@@ -6306,7 +6285,7 @@
         <v>437</v>
       </c>
       <c r="C363" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.35">
@@ -6317,7 +6296,7 @@
         <v>439</v>
       </c>
       <c r="C364" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.35">
@@ -6328,7 +6307,7 @@
         <v>440</v>
       </c>
       <c r="C365" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.35">
@@ -6339,7 +6318,7 @@
         <v>441</v>
       </c>
       <c r="C366" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.35">
@@ -6350,7 +6329,7 @@
         <v>442</v>
       </c>
       <c r="C367" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.35">
@@ -6361,7 +6340,7 @@
         <v>443</v>
       </c>
       <c r="C368" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.35">
@@ -6372,7 +6351,7 @@
         <v>444</v>
       </c>
       <c r="C369" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.35">
@@ -6383,7 +6362,7 @@
         <v>445</v>
       </c>
       <c r="C370" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.35">
@@ -6394,7 +6373,7 @@
         <v>446</v>
       </c>
       <c r="C371" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.35">
@@ -6405,7 +6384,7 @@
         <v>447</v>
       </c>
       <c r="C372" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.35">
@@ -6416,7 +6395,7 @@
         <v>449</v>
       </c>
       <c r="C373" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.35">
@@ -6427,7 +6406,7 @@
         <v>450</v>
       </c>
       <c r="C374" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.35">
@@ -6438,7 +6417,7 @@
         <v>451</v>
       </c>
       <c r="C375" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.35">
@@ -6449,7 +6428,7 @@
         <v>452</v>
       </c>
       <c r="C376" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.35">
@@ -6460,7 +6439,7 @@
         <v>453</v>
       </c>
       <c r="C377" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.35">
@@ -6471,7 +6450,7 @@
         <v>454</v>
       </c>
       <c r="C378" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.35">
@@ -6498,7 +6477,7 @@
         <v>457</v>
       </c>
       <c r="C381" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.35">
@@ -6509,7 +6488,7 @@
         <v>458</v>
       </c>
       <c r="C382" t="s">
-        <v>756</v>
+        <v>751</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.35">
@@ -6536,7 +6515,7 @@
         <v>461</v>
       </c>
       <c r="C385" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.35">
@@ -6555,7 +6534,7 @@
         <v>464</v>
       </c>
       <c r="C387" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.35">
@@ -6574,7 +6553,7 @@
         <v>466</v>
       </c>
       <c r="C389" t="s">
-        <v>759</v>
+        <v>754</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.35">
@@ -6593,7 +6572,7 @@
         <v>468</v>
       </c>
       <c r="C391" t="s">
-        <v>760</v>
+        <v>755</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.35">
@@ -6612,7 +6591,7 @@
         <v>470</v>
       </c>
       <c r="C393" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.35">
@@ -6623,7 +6602,7 @@
         <v>471</v>
       </c>
       <c r="C394" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.35">
@@ -6634,7 +6613,7 @@
         <v>473</v>
       </c>
       <c r="C395" t="s">
-        <v>763</v>
+        <v>758</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.35">
@@ -6669,7 +6648,7 @@
         <v>477</v>
       </c>
       <c r="C399" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.35">
@@ -6688,7 +6667,7 @@
         <v>479</v>
       </c>
       <c r="C401" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.35">
@@ -6699,7 +6678,7 @@
         <v>480</v>
       </c>
       <c r="C402" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.35">
@@ -6710,7 +6689,7 @@
         <v>482</v>
       </c>
       <c r="C403" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.35">
@@ -6737,7 +6716,7 @@
         <v>485</v>
       </c>
       <c r="C406" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.35">
@@ -6748,7 +6727,7 @@
         <v>486</v>
       </c>
       <c r="C407" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.35">
@@ -6767,7 +6746,7 @@
         <v>488</v>
       </c>
       <c r="C409" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.35">
@@ -6826,7 +6805,7 @@
         <v>495</v>
       </c>
       <c r="C416" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.35">
@@ -6837,7 +6816,7 @@
         <v>497</v>
       </c>
       <c r="C417" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.35">
@@ -6848,7 +6827,7 @@
         <v>498</v>
       </c>
       <c r="C418" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.35">
@@ -6859,7 +6838,7 @@
         <v>499</v>
       </c>
       <c r="C419" t="s">
-        <v>775</v>
+        <v>770</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.35">
@@ -6878,7 +6857,7 @@
         <v>501</v>
       </c>
       <c r="C421" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.35">
@@ -6897,7 +6876,7 @@
         <v>503</v>
       </c>
       <c r="C423" t="s">
-        <v>777</v>
+        <v>772</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.35">
@@ -6916,7 +6895,7 @@
         <v>506</v>
       </c>
       <c r="C425" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.35">
@@ -6927,7 +6906,7 @@
         <v>507</v>
       </c>
       <c r="C426" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.35">
@@ -6938,7 +6917,7 @@
         <v>508</v>
       </c>
       <c r="C427" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.35">
@@ -6949,7 +6928,7 @@
         <v>509</v>
       </c>
       <c r="C428" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.35">
@@ -6968,7 +6947,7 @@
         <v>511</v>
       </c>
       <c r="C430" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.35">
@@ -6979,7 +6958,7 @@
         <v>512</v>
       </c>
       <c r="C431" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.35">
@@ -6990,7 +6969,7 @@
         <v>513</v>
       </c>
       <c r="C432" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.35">
@@ -7001,7 +6980,7 @@
         <v>514</v>
       </c>
       <c r="C433" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.35">
@@ -7123,9 +7102,6 @@
       <c r="B445" t="s">
         <v>13</v>
       </c>
-      <c r="C445" t="s">
-        <v>526</v>
-      </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A446">
@@ -7135,7 +7111,7 @@
         <v>14</v>
       </c>
       <c r="C446" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.35">
@@ -7210,7 +7186,7 @@
         <v>24</v>
       </c>
       <c r="C455" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.35">
@@ -7220,9 +7196,6 @@
       <c r="B456" t="s">
         <v>26</v>
       </c>
-      <c r="C456" t="s">
-        <v>529</v>
-      </c>
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A457">
@@ -7232,7 +7205,7 @@
         <v>27</v>
       </c>
       <c r="C457" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.35">
@@ -7243,7 +7216,7 @@
         <v>28</v>
       </c>
       <c r="C458" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.35">
@@ -7270,7 +7243,7 @@
         <v>31</v>
       </c>
       <c r="C461" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.35">
@@ -7281,7 +7254,7 @@
         <v>32</v>
       </c>
       <c r="C462" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.35">
@@ -7300,7 +7273,7 @@
         <v>34</v>
       </c>
       <c r="C464" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.35">
@@ -7319,7 +7292,7 @@
         <v>37</v>
       </c>
       <c r="C466" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.35">
@@ -7330,7 +7303,7 @@
         <v>38</v>
       </c>
       <c r="C467" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.35">
@@ -7357,7 +7330,7 @@
         <v>41</v>
       </c>
       <c r="C470" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.35">
@@ -7376,7 +7349,7 @@
         <v>43</v>
       </c>
       <c r="C472" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.35">
@@ -7387,7 +7360,7 @@
         <v>44</v>
       </c>
       <c r="C473" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.35">
@@ -7406,7 +7379,7 @@
         <v>46</v>
       </c>
       <c r="C475" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.35">
@@ -7417,7 +7390,7 @@
         <v>47</v>
       </c>
       <c r="C476" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.35">
@@ -7436,7 +7409,7 @@
         <v>50</v>
       </c>
       <c r="C478" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.35">
@@ -7447,7 +7420,7 @@
         <v>51</v>
       </c>
       <c r="C479" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.35">
@@ -7458,7 +7431,7 @@
         <v>52</v>
       </c>
       <c r="C480" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.35">
@@ -7469,7 +7442,7 @@
         <v>53</v>
       </c>
       <c r="C481" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.35">
@@ -7496,7 +7469,7 @@
         <v>56</v>
       </c>
       <c r="C484" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.35">
@@ -7539,7 +7512,7 @@
         <v>62</v>
       </c>
       <c r="C489" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.35">
@@ -7550,7 +7523,7 @@
         <v>63</v>
       </c>
       <c r="C490" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.35">
@@ -7561,7 +7534,7 @@
         <v>64</v>
       </c>
       <c r="C491" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.35">
@@ -7572,7 +7545,7 @@
         <v>65</v>
       </c>
       <c r="C492" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.35">
@@ -7583,7 +7556,7 @@
         <v>66</v>
       </c>
       <c r="C493" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.35">
@@ -7594,7 +7567,7 @@
         <v>67</v>
       </c>
       <c r="C494" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.35">
@@ -7637,7 +7610,7 @@
         <v>73</v>
       </c>
       <c r="C499" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.35">
@@ -7656,7 +7629,7 @@
         <v>75</v>
       </c>
       <c r="C501" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.35">
@@ -7667,7 +7640,7 @@
         <v>76</v>
       </c>
       <c r="C502" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.35">
@@ -7678,7 +7651,7 @@
         <v>77</v>
       </c>
       <c r="C503" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.35">
@@ -7689,7 +7662,7 @@
         <v>78</v>
       </c>
       <c r="C504" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.35">
@@ -7716,7 +7689,7 @@
         <v>81</v>
       </c>
       <c r="C507" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.35">
@@ -7727,7 +7700,7 @@
         <v>83</v>
       </c>
       <c r="C508" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.35">
@@ -7738,7 +7711,7 @@
         <v>84</v>
       </c>
       <c r="C509" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.35">
@@ -7757,7 +7730,7 @@
         <v>86</v>
       </c>
       <c r="C511" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.35">
@@ -7768,7 +7741,7 @@
         <v>87</v>
       </c>
       <c r="C512" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.35">
@@ -7779,7 +7752,7 @@
         <v>88</v>
       </c>
       <c r="C513" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="514" spans="1:3" x14ac:dyDescent="0.35">
@@ -7798,7 +7771,7 @@
         <v>90</v>
       </c>
       <c r="C515" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.35">
@@ -7809,7 +7782,7 @@
         <v>92</v>
       </c>
       <c r="C516" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed the clean text function to ractify data loss
</commit_message>
<xml_diff>
--- a/Screenshots/pilot_ep_1.xlsx
+++ b/Screenshots/pilot_ep_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\linux\scratches\Netflix_image_subtitle_crawler\Screenshots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76902CA3-29EF-4EE8-86C8-E0E2E9F6CEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B730595D-19E1-47FD-9F6F-144E38F08D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6700" yWindow="-50" windowWidth="14400" windowHeight="7030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="784">
   <si>
     <t>time(sec)</t>
   </si>
@@ -1582,13 +1582,13 @@
     <t>अधिकांश औरतें वील नहीं खातीं।</t>
   </si>
   <si>
-    <t>तुमसे बात करने की कोशिश भी क्‍यों करता हूँ?</t>
-  </si>
-  <si>
-    <t>छोड़ो भी, मैं तुम्हें हल्का करने की कोशिश कर रहा हूँ।</t>
-  </si>
-  <si>
-    <t>मुझे हल्का होने की ज़रूरत नहीं मेरी दुनिया में अंधेरा है।</t>
+    <t>तुमसे बात करने की  कोशिश भी क्‍यों करता हूँ?</t>
+  </si>
+  <si>
+    <t>छोड़ो भी, मैं तुम्हें  हल्का करने की कोशिश कर रहा हूँ।</t>
+  </si>
+  <si>
+    <t>मुझे हल्का होने की ज़रूरत नहीं  मेरी दुनिया में अंधेरा है।</t>
   </si>
   <si>
     <t>अंधेरा और बरसाती।</t>
@@ -1597,7 +1597,7 @@
     <t>और तुम इसमें बेकार हो!</t>
   </si>
   <si>
-    <t>सच में? मैं उस समय बेकार नहीं था जब तुम्हें रहने के लिए जगह चाहिए थी।</t>
+    <t>सच में? मैं उस समय बेकार नहीं था  जब तुम्हें रहने के लिए जगह चाहिए थी।</t>
   </si>
   <si>
     <t>बेशक, वह एक गलती थी।</t>
@@ -1609,13 +1609,13 @@
     <t>क्या हो रहा है? नींद नहीं आई?</t>
   </si>
   <si>
-    <t>मेरे डैड ने कहा हम कल दादी माँ के घर जा रहे हैं।</t>
+    <t>मेरे डैड ने कहा  हम कल दादी माँ के घर जा रहे हैं।</t>
   </si>
   <si>
     <t>हाँ, इसी ने मुझे भी जगाए रखा।</t>
   </si>
   <si>
-    <t>अगर इससे कुछ बेहतर महसूस हो तो तुम आखिरी बाज़ी में डॉलर जीते।</t>
+    <t>अगर इससे कुछ बेहतर महसूस हो  तो तुम आखिरी बाज़ी में 80 डॉलर जीते।</t>
   </si>
   <si>
     <t>पचासी डॉलर।</t>
@@ -1624,10 +1624,10 @@
     <t>काश मेरे डैड आप जैसे मस्त होते।</t>
   </si>
   <si>
-    <t>वह दुनिया में तुम्हें सबसे बढ़कर प्यार करते हैं।</t>
-  </si>
-  <si>
-    <t>तुम यह जानते हो, है</t>
+    <t>वह दुनिया में तुम्हें  सबसे बढ़कर प्यार करते हैं।</t>
+  </si>
+  <si>
+    <t>तुम यह जानते हो, है न?</t>
   </si>
   <si>
     <t>आपके कोई बच्चा क्‍यों नहीं है?</t>
@@ -1636,16 +1636,16 @@
     <t>मुझे नहीं पता।</t>
   </si>
   <si>
-    <t>शायद मैं इस दुनिया में सबसे अधिक खुद से प्यार करता हूँ।</t>
-  </si>
-  <si>
-    <t>चार्ली?</t>
+    <t>शायद मैं इस दुनिया में  सबसे अधिक खुद से प्यार करता हूँ।</t>
+  </si>
+  <si>
+    <t>-अंकल  चार्ली?  -हॉा? द</t>
   </si>
   <si>
     <t>मुझे दादी माँ के घर नहीं जाना। यहाँ रहना है।</t>
   </si>
   <si>
-    <t>हाँ, तुम्हारे डैड जानते हैं कि तुम्हारे लिए क्‍या सही है।</t>
+    <t>हाँ, तुम्हारे डैड जानते हैं  कि तुम्हारे लिए क्‍या सही है।</t>
   </si>
   <si>
     <t>ठीक है। गुड नाइट, अंकल चार्ली।</t>
@@ -1654,7 +1654,7 @@
     <t>ठीक है।</t>
   </si>
   <si>
-    <t>यह रुकेगी? क्‍योंकि मैंने अपनी कार इसकी कार के पीछे लगाई है।</t>
+    <t>यह रुकेगी? क्‍योंकि मैंने  अपनी कार इसकी कार के पीछे लगाई है।</t>
   </si>
   <si>
     <t>उस जैसे बच्चे से प्यार हो जाता है।</t>
@@ -1663,7 +1663,7 @@
     <t>उसके लिए स्टेयरवे टू हेवन भी बजाया,</t>
   </si>
   <si>
-    <t>और फिर भी उसे मेपल लूप्स गाना अधिक पसंद आया।</t>
+    <t>और फिर भी उसे  मेपल लूप्स गाना अधिक पसंद आया।</t>
   </si>
   <si>
     <t>मैं तुमसे दो हफ़्ते से नहीं मिली हूँ।</t>
@@ -1672,22 +1672,22 @@
     <t>तुम्हें अपना घर वापस मिल गया।</t>
   </si>
   <si>
-    <t>तुम्हें अपने भतीजे के बारे में बात करनी है, या सेक्स करना है?</t>
-  </si>
-  <si>
-    <t>कुछ हर है।</t>
-  </si>
-  <si>
-    <t>वाह, हमारी बढ़िया जम रही है। क्या हम इसी तक रहने दें?</t>
-  </si>
-  <si>
-    <t>तुम क्या कर रही हो? मुझे लगा हम सेक्स करने वाले थे।</t>
-  </si>
-  <si>
-    <t>मैं कैसे सेक्‍स करूँ जबकि तुम बच्चे पैदा करने के बारे में सोच रहे हो?</t>
-  </si>
-  <si>
-    <t>हेलो, चार्ली बोल रहा हूँ। बीप की आवाज़ सुनते ही अपनी बात कहें।</t>
+    <t>तुम्हें अपने भतीजे के बारे में  बात करनी है, या सेक्स करना है?</t>
+  </si>
+  <si>
+    <t>-तुमसे  कुछ [छना  हर है।</t>
+  </si>
+  <si>
+    <t>वाह, हमारी बढ़िया जम रही है।  क्या हम इसी तक न रहने दें?</t>
+  </si>
+  <si>
+    <t>तुम क्या कर रही हो?  मुझे लगा हम सेक्स करने वाले थे।</t>
+  </si>
+  <si>
+    <t>मैं कैसे सेक्‍स करूँ जबकि तुम  बच्चे पैदा करने के बारे में सोच रहे हो?</t>
+  </si>
+  <si>
+    <t>हेलो, चार्ली बोल रहा हूँ।  बीप की आवाज़ सुनते ही अपनी बात कहें।</t>
   </si>
   <si>
     <t>हेलो, मंकी मैन।</t>
@@ -1696,16 +1696,16 @@
     <t>मैं तुम्हारे बारे में सोच रही थी,</t>
   </si>
   <si>
-    <t>और जानना था कि हम एक-दूसरे को इतना दुख क्‍यों देते हैं।</t>
+    <t>और जानना था कि हम एक-दूसरे को  इतना दुख क्‍यों देते हैं।</t>
   </si>
   <si>
     <t>रोज़, मैं बोल रहा हूँ, मंकी मैन।</t>
   </si>
   <si>
-    <t>सुनो, तुमसे एक सवाल पूछना है।</t>
-  </si>
-  <si>
-    <t>किसी औरत से यह पूछना स्वाभाविक तौर पर गलत है</t>
+    <t>-चार्ली?  -हाँ, सुनो, तुमसे एक सवाल पूछना है।</t>
+  </si>
+  <si>
+    <t>किसी औरत से यह पूछना  स्वाभाविक तौर पर गलत है</t>
   </si>
   <si>
     <t>यह हम दोनों के लिए है। जाना मत।</t>
@@ -1717,40 +1717,40 @@
     <t>मतलब, शादी की कसमों का क्या मतलब?</t>
   </si>
   <si>
-    <t>पता है, दम तक।" कौन मरा? मैं। और ही वह।</t>
+    <t>पता है, "मरते दम तक।"  कौन मरा? न मैं। और न ही वह।</t>
   </si>
   <si>
     <t>तुम मेरे घर में अंदर कैसे आए?</t>
   </si>
   <si>
-    <t>अच्छा, चार्ली, नकली पत्थर में चाबी तभी छिपती है जब दूसरे पत्थर साथ में हों।</t>
-  </si>
-  <si>
-    <t>कि तुम्हारे पायदान पर हो।</t>
-  </si>
-  <si>
-    <t>माफ़ करना, पर अगर तुम नकली पत्थर को दूसरे पत्थरों के ढेर में रखोगे</t>
-  </si>
-  <si>
-    <t>तो नशे की हालत में उसे ढूँढना कठिन होगा।</t>
-  </si>
-  <si>
-    <t>चिंता मत करो। मेरे पैरों में इतना खून नहीं बचा कि कहीं और जा सकू।</t>
+    <t>अच्छा, चार्ली, नकली पत्थर में चाबी  तभी छिपती है जब दूसरे पत्थर साथ में हों।</t>
+  </si>
+  <si>
+    <t>न कि तुम्हारे पायदान पर हो।</t>
+  </si>
+  <si>
+    <t>माफ़ करना, पर अगर तुम नकली पत्थर को  दूसरे पत्थरों के ढेर में रखोगे</t>
+  </si>
+  <si>
+    <t>तो नशे की हालत में  उसे ढूँढना कठिन होगा।</t>
+  </si>
+  <si>
+    <t>चिंता मत करो। मेरे पैरों में  इतना खून नहीं बचा कि कहीं और जा सकू।</t>
   </si>
   <si>
     <t>मैं एक अच्छा पति हूँ। भरोसेमंद हूँ।</t>
   </si>
   <si>
-    <t>बेहूदा मत बनो। जूड़िथ को सेक्स भी पसंद नहीं।</t>
-  </si>
-  <si>
-    <t>मतलब, वह कहती रहती दम घुट रहा है, पता है?</t>
-  </si>
-  <si>
-    <t>वह बोलती रहती, दम घुट रहा है।"</t>
-  </si>
-  <si>
-    <t>इसका क्या मतलब है, क्या किसी औरत ने तुमसे कभी कहा?</t>
+    <t>बेहूदा मत बनो।  जूड़िथ को सेक्स भी पसंद नहीं।</t>
+  </si>
+  <si>
+    <t>मतलब, वह कहती रहती  दम घुट रहा है, पता है?</t>
+  </si>
+  <si>
+    <t>वह बोलती रहती, "मैरा दम घुट रहा है।"</t>
+  </si>
+  <si>
+    <t>इसका क्या मतलब है,  क्या किसी औरत ने तुमसे कभी कहा?</t>
   </si>
   <si>
     <t>ख़ैर, हाँ।</t>
@@ -1762,28 +1762,28 @@
     <t>और जेक। इससे जेक बस बर्बाद हो जाएगा।</t>
   </si>
   <si>
-    <t>बेटा।</t>
+    <t>-जेक?  -मेरा बेटा।</t>
   </si>
   <si>
     <t>इन दिनों किशोर काफ़ी विवेकशील होते हैं।</t>
   </si>
   <si>
-    <t>मैं जा रही हूँ।</t>
+    <t>-चार्ली, मैं जा रही हूँ।  -नहीं।</t>
   </si>
   <si>
     <t>तुम दोनों बात करो। कल फ़ोन करूँगी।</t>
   </si>
   <si>
-    <t>तुम तुम्हारी पत्नी का सुनकर दुख हुआ।</t>
-  </si>
-  <si>
-    <t>छोड़ो, तुम्हारे जाने से ये कौन से साथ रहने लगेंगे।</t>
+    <t>तुम व तुम्हारी पत्नी का सुनकर दुख हुआ।</t>
+  </si>
+  <si>
+    <t>छोड़ो, तुम्हारे जाने से  ये कौन से साथ रहने लगेंगे।</t>
   </si>
   <si>
     <t>यह तब तक है जब तक हालात सुधरते नहीं।</t>
   </si>
   <si>
-    <t>अधिक से अधिक कुछ दिन। उसका दिमाग ठिकाने जाएगा।</t>
+    <t>अधिक से अधिक कुछ दिन।  उसका दिमाग ठिकाने आ जाएगा।</t>
   </si>
   <si>
     <t>हा। औरतें यही करती हैं।</t>
@@ -1798,7 +1798,7 @@
     <t>मुझे अपनी चादरें पसंद हैं।</t>
   </si>
   <si>
-    <t>है, फ़िर, गुड नाइट। रुको।</t>
+    <t>-ठीक है, फ़िर, गुड नाइट।  -नहीं, रुको।</t>
   </si>
   <si>
     <t>हम मुश्किल से एक-दूसरे से बात करते हैं।</t>
@@ -1810,10 +1810,10 @@
     <t>सैन फर्नाडो वैली काइरोप्रैक्टिक संघ ने</t>
   </si>
   <si>
-    <t>मुझे काइरोप्रैक्टर ऑफ़ ईयर नामित किया।</t>
-  </si>
-  <si>
-    <t>है, फ़िर। गुड नाइट।</t>
+    <t>मुझे काइरोप्रैक्टर ऑफ़ द ईयर नामित किया।</t>
+  </si>
+  <si>
+    <t>-ठीक है, फ़िर। गुड नाइट।  -नहीं।</t>
   </si>
   <si>
     <t>अपने बारे में बताओ?</t>
@@ -1825,22 +1825,22 @@
     <t>मैं थोड़ा सा काम करके काफ़ी पैसे बनाता हूँ।</t>
   </si>
   <si>
-    <t>सुंदर औरतों साथ सोता हूँ जिन्हें मेरी भावनाओं से मतलब नहीं।</t>
+    <t>सुंदर औरतों साथ सोता हूँ  जिन्हें मेरी भावनाओं से मतलब नहीं।</t>
   </si>
   <si>
     <t>जैगुआर चलाता और बीच पर रहता हूँ,</t>
   </si>
   <si>
-    <t>और कभी-कभी दिन के बीच में, बिना किसी वजह के,</t>
+    <t>और कभी-कभी दिन के बीच में,  बिना किसी वजह के,</t>
   </si>
   <si>
     <t>अपने लिए मार्गरीटा का बड़ा जग बनाता हूँ,</t>
   </si>
   <si>
-    <t>है। गुड नाइट, चार्ली। नाइट।</t>
-  </si>
-  <si>
-    <t>सुनो, घटिया इंसान, मैं अपने साथ ऐसा बर्ताव नहीं होने टूँगी।</t>
+    <t>-ठीक है। गुड नाइट, चार्ली।  -गुड नाइट।</t>
+  </si>
+  <si>
+    <t>सुनो, घटिया इंसान,  मैं अपने साथ ऐसा बर्ताव नहीं होने टूँगी।</t>
   </si>
   <si>
     <t>अरे, आपकी आँखें लाल हैं।</t>
@@ -1855,61 +1855,61 @@
     <t>मुझे समुद्र में तैरने ले चलेंगे?</t>
   </si>
   <si>
-    <t>मेरा सिरदर्द ख़त्म होने के बाद इस पर बात करें?</t>
-  </si>
-  <si>
-    <t>या तो मुझे फ़ोन करो, या तुम्हें बहुत अफ़सोस होने वाला है।</t>
+    <t>मेरा सिरदर्द ख़त्म होने के बाद  इस पर बात करें?</t>
+  </si>
+  <si>
+    <t>या तो मुझे फ़ोन करो,  या तुम्हें बहुत अफ़सोस होने वाला है।</t>
   </si>
   <si>
     <t>ख़ैर, मैंने कल रात थोड़ी ज़्यादा वाइन पी ली।</t>
   </si>
   <si>
-    <t>अगर इससे आपकी तबीयत ख़राब होती है, तो क्यों पीते हैं?</t>
+    <t>अगर इससे आपकी तबीयत ख़राब होती है,  तो क्यों पीते हैं?</t>
   </si>
   <si>
     <t>किसी को चंट गधे पसंद नहीं।</t>
   </si>
   <si>
-    <t>आपको एक डॉलर गाली वाले जार में डालना होगा क्योंकि आपने बोला।</t>
+    <t>आपको एक डॉलर गाली वाले जार में  डालना होगा क्योंकि आपने "गधा" बोला।</t>
   </si>
   <si>
     <t>तुम्हें बताता हूँ,</t>
   </si>
   <si>
-    <t>यह लो डॉलर। अब से लेकर लंच के लिए हैं।</t>
+    <t>यह लो 20 डॉलर।  अब से लेकर लंच के लिए हैं।</t>
   </si>
   <si>
     <t>अब, मुझे लगता है कि तुम एक सूची बनाओ।</t>
   </si>
   <si>
-    <t>एक ओर लिखो, हमारी शादी के बारे में क्या नापसंद है,</t>
+    <t>एक ओर लिखो,  हमारी शादी के बारे में क्या नापसंद है,</t>
   </si>
   <si>
     <t>और दूसरी ओर, तुम्हें जो पसंद है।</t>
   </si>
   <si>
-    <t>कभी-कभी जब तुम्हारे पास घर आने का सोचती हूँ,</t>
+    <t>कभी-कभी जब  तुम्हारे पास घर आने का सोचती हूँ,</t>
   </si>
   <si>
     <t>तो कार में ही रोने लगती हूँ।</t>
   </si>
   <si>
-    <t>ठीक है, तो यह शायद की ओर रहेगा।</t>
+    <t>ठीक है, तो यह शायद "न" की ओर रहेगा।</t>
   </si>
   <si>
     <t>मैं झूठ क्यों बोलँगा? आज समुद्र बंद है।</t>
   </si>
   <si>
-    <t>है राम, तुम्हें नहीं लगता कि तुम पैंट पहन लो?</t>
-  </si>
-  <si>
-    <t>मुझे देखो, जूडी। मुझे पैंट पहनने का समय नहीं मिला।</t>
-  </si>
-  <si>
-    <t>हाँ, आओ, बच्चे, हम बाहर छत पर नाश्ता करेंगे।</t>
-  </si>
-  <si>
-    <t>लंच करेंगे। लंच का समय नहीं।</t>
+    <t>है राम, तुम्हें नहीं लगता  कि तुम पैंट पहन लो?</t>
+  </si>
+  <si>
+    <t>मुझे देखो, जूडी।  मुझे पैंट पहनने का समय नहीं मिला।</t>
+  </si>
+  <si>
+    <t>हाँ, आओ, बच्चे,  हम बाहर छत पर नाश्ता करेंगे।</t>
+  </si>
+  <si>
+    <t>-अच्छा, लंच करेंगे।  -यह लंच का समय नहीं।</t>
   </si>
   <si>
     <t>जूडिथ, मैं बदल सकता हूँ।</t>
@@ -1933,10 +1933,10 @@
     <t>हाँ। यह ऐसा लगता तो है।</t>
   </si>
   <si>
-    <t>तुम्हारी उम्र में अपने माँ-बाप के अलग होने का सपना ही देख सका।</t>
-  </si>
-  <si>
-    <t>दादी माँ कहती हैं आपने बहुत निराश किया।</t>
+    <t>तुम्हारी उम्र में अपने माँ-बाप  के अलग होने का सपना ही देख सका।</t>
+  </si>
+  <si>
+    <t>दादी माँ कहती हैं  आपने बहुत निराश किया।</t>
   </si>
   <si>
     <t>सुनो, तुम्हारी माँ अलविदा कहना चाहती हैं।</t>
@@ -1945,13 +1945,13 @@
     <t>सुनो, वह कुछ नहीं जानता जो भी चल रहा है,</t>
   </si>
   <si>
-    <t>हमारा छोटा सा राज़। वह उसे अलविदा क्यों कह रही है?</t>
-  </si>
-  <si>
-    <t>एक टेलीमार्केटर जो मंकी मैन कहकर बुलाती है?</t>
-  </si>
-  <si>
-    <t>वह वेगास में अपनी बहन के साथ सप्ताहांत बिताने जा रही है।</t>
+    <t>हमारा छोटा सा राज़।  वह उसे अलविदा क्यों कह रही है?</t>
+  </si>
+  <si>
+    <t>एक टेलीमार्केटर  जो मंकी मैन कहकर बुलाती है?</t>
+  </si>
+  <si>
+    <t>वह वेगास में अपनी बहन के साथ  सप्ताहांत बिताने जा रही है।</t>
   </si>
   <si>
     <t>तो, हमने तय किया कि जेक मेरे साथ रहेगा।</t>
@@ -1963,12 +1963,15 @@
     <t>मैं कुछ अजीब सूची में हूँ।</t>
   </si>
   <si>
-    <t>शुक्रिया। सुनो, मुझे दफ़्तर में फ़ोन करना है।</t>
+    <t>शुक्रिया। सुनो,  मुझे दफ़्तर में फ़ोन करना है।</t>
   </si>
   <si>
     <t>इसके लिए लंच बना दोगे?</t>
   </si>
   <si>
+    <t>-ज़रूर।  -शुक्रिया।</t>
+  </si>
+  <si>
     <t>तुम क्यों मुस्करा रहे हो?</t>
   </si>
   <si>
@@ -1981,7 +1984,7 @@
     <t>अब कौन मुस्करा रहा है?</t>
   </si>
   <si>
-    <t>दूध पीते हो? के साथ।</t>
+    <t>-तुम दूध पीते हो?  -कॉर्नफ्लेक्स के साथ।</t>
   </si>
   <si>
     <t>तो, तुम्हें कैसा लगा?</t>
@@ -1990,7 +1993,7 @@
     <t>यह वाला दूध नहीं, वह वाला दूध।</t>
   </si>
   <si>
-    <t>फ़र्क पड़ता है? डेयरी फ़ार्म है। हम डेयरी बार्न पीते हैं।</t>
+    <t>-क्या फ़र्क पड़ता है?  -यह डेयरी फ़ार्म है। हम डेयरी बार्न पीते हैं।</t>
   </si>
   <si>
     <t>बढ़िया।</t>
@@ -1999,16 +2002,16 @@
     <t>मैं क्यों खुश होऊँगा? यह बस दूध है।</t>
   </si>
   <si>
-    <t>अच्छा, यह एक औरत है जिसके साथ एक बार बाहर गया और वह थोड़ी चिपकू हो गई।</t>
-  </si>
-  <si>
-    <t>होशियार होौ। लगे रहो। तुम उनमें से एक कार्टन पर होगे।</t>
+    <t>अच्छा, यह एक औरत है जिसके साथ एक बार  बाहर गया और वह थोड़ी चिपकू हो गई।</t>
+  </si>
+  <si>
+    <t>होशियार होौ। लगे रहो।  तुम उनमें से एक कार्टन पर होगे।</t>
   </si>
   <si>
     <t>ठीक है, कॉर्नफ्लेक्स।</t>
   </si>
   <si>
-    <t>हमारे पास लकी चार्म्स, कोको पफ़्स, फ्रोस्टेड फ़्लेक्स, मेपल लूप्स।</t>
+    <t>हमारे पास लकी चार्म्स,  कोको पफ़्स, फ्रोस्टेड फ़्लेक्स, मेपल लूप्स।</t>
   </si>
   <si>
     <t>इसमें ओट्स, मक्का और गेहूँ है</t>
@@ -2023,13 +2026,13 @@
     <t>पता है यह गाना किसने लिखा?</t>
   </si>
   <si>
-    <t>चार्ली ने लिखा। नहीं?</t>
-  </si>
-  <si>
-    <t>अगर झूठ बोलना होता तो कहता स्टेयरवे ट्‌ हेवन लिखा,</t>
-  </si>
-  <si>
-    <t>लोगों की खूब बनती है।</t>
+    <t>-अंकल चार्ली ने लिखा।  -झूठ नहीं?</t>
+  </si>
+  <si>
+    <t>अगर झूठ बोलना होता तो कहता  स्टेयरवे ट्‌ हेवन लिखा,</t>
+  </si>
+  <si>
+    <t>-तुम लोगों की खूब बनती है।  -शुक्रिया।</t>
   </si>
   <si>
     <t>तुम एक बहुत खराब लड़के हो।</t>
@@ -2041,10 +2044,10 @@
     <t>डॉ. ब्लूम? हाँ, एलन हार्पर बोल रहा हूँ।</t>
   </si>
   <si>
-    <t>मेरी पत्नी मैं दोपहर की हमारी शादी के परामर्श की अपॉइंटमेंट रद्द करना चाहते हैं।</t>
-  </si>
-  <si>
-    <t>हाँ, ख़ैर, कुछ काम गया।</t>
+    <t>मेरी पत्नी व मैं दोपहर की हमारी शादी के  परामर्श की अपॉइंटमेंट रद्द करना चाहते हैं।</t>
+  </si>
+  <si>
+    <t>हाँ, ख़ैर, कुछ काम आ गया।</t>
   </si>
   <si>
     <t>ख़ेर, यह थोडा निजी है। मेरा मतलब</t>
@@ -2056,10 +2059,10 @@
     <t>हाँ, इन बातों की अहमियत जानता हूँ--</t>
   </si>
   <si>
-    <t>चार्ली घर पर है?</t>
-  </si>
-  <si>
-    <t>नहीं। मैं चार्ली का भाई हूँ। क्या मदद कर सकता हूँ?</t>
+    <t>-हेलो?  -क्या चार्ली घर पर है?</t>
+  </si>
+  <si>
+    <t>नहीं। मैं चार्ली का भाई हूँ।  क्या मदद कर सकता हूँ?</t>
   </si>
   <si>
     <t>हेलो, चार्ली के भाई। मैं रोज़ हूँ।</t>
@@ -2074,10 +2077,10 @@
     <t>मैं अपने बिलों के भुगतान के लिए करती हूँ।</t>
   </si>
   <si>
-    <t>किसकी खुशबू रही है?</t>
-  </si>
-  <si>
-    <t>तुम्हारे भाई की। उसकी महक कस्तूरी की खुशबू जैसी है।</t>
+    <t>किसकी खुशबू आ रही है?</t>
+  </si>
+  <si>
+    <t>तुम्हारे भाई की।  उसकी महक कस्तूरी की खुशबू जैसी है।</t>
   </si>
   <si>
     <t>ख़ैर, तुम अपना काम करो।</t>
@@ -2092,55 +2095,55 @@
     <t>तुम्हें इतनी देर क्यों लगी?</t>
   </si>
   <si>
-    <t>हम आइसक्रीम के लिए रुके क्योंकि मैं औरतों को आकृष्ट करता हूँ।</t>
+    <t>हम आइसक्रीम के लिए रुके  क्योंकि मैं औरतों को आकृष्ट करता हूँ।</t>
   </si>
   <si>
     <t>मुझे सु-सु जाना है।</t>
   </si>
   <si>
-    <t>हेलो, चार्ली बोल रहा हूँ। बीप की आवाज़ पर अपनी बात कहें।</t>
-  </si>
-  <si>
-    <t>यह क्‍यों मान रहे हो कि उसने मुझसे सीखा?</t>
-  </si>
-  <si>
-    <t>के लिए शुक्रिया। मैंने नहीं की। रोज़ आई थी।</t>
+    <t>हेलो, चार्ली बोल रहा हूँ।  बीप की आवाज़ पर अपनी बात कहें।</t>
+  </si>
+  <si>
+    <t>यह क्‍यों मान रहे हो  कि उसने मुझसे सीखा?</t>
+  </si>
+  <si>
+    <t>-सफ़ाई के लिए शुक्रिया।  -नहीं, मैंने नहीं की। रोज़ आई थी।</t>
   </si>
   <si>
     <t>रोज़? तुमने रोज़ को मेरे घर में आने दिया?</t>
   </si>
   <si>
-    <t>उसने फ़िर से कैबिनेट को गोंद से चिपका दिया।</t>
+    <t>उसने फ़िर से कैबिनेट  को गोंद से चिपका दिया।</t>
   </si>
   <si>
     <t>फ़िर से?</t>
   </si>
   <si>
-    <t>कोई ऐसा है जो कैबिनेट को गोंद से चिपकाने आता है?</t>
-  </si>
-  <si>
-    <t>कुछ पागल लोगों से मिले हो जिनके साथ मैं घूमता हूँ।</t>
-  </si>
-  <si>
-    <t>सकते हो कि रोज़ कैसी है। यह मेरी गलती है?</t>
-  </si>
-  <si>
-    <t>तुम काफ़ी परेशान इंसान हो, पता है? हटो। चलो।</t>
+    <t>कोई ऐसा है जो कैबिनेट को  गोंद से चिपकाने आता है?</t>
+  </si>
+  <si>
+    <t>कुछ पागल लोगों से मिले हो  जिनके साथ मैं घूमता हूँ।</t>
+  </si>
+  <si>
+    <t>-सोच सकते हो कि रोज़ कैसी है।  -तो, यह मेरी गलती है?</t>
+  </si>
+  <si>
+    <t>तुम काफ़ी परेशान इंसान हो,  पता है? हटो। चलो।</t>
   </si>
   <si>
     <t>मैं काफ़ी परेशान इंसान हूँ?</t>
   </si>
   <si>
-    <t>यहाँ कौन आधी रात को अपनी खुद की चादर के साथ आया?</t>
-  </si>
-  <si>
-    <t>कम से कम परवाह है कि किस पर सोता हूँ। या कहना चाहिए, किसके साथ सोता हूँ।</t>
+    <t>यहाँ कौन आधी रात को  अपनी खुद की चादर के साथ आया?</t>
+  </si>
+  <si>
+    <t>कम से कम परवाह है कि किस पर सोता हूँ।  या कहना चाहिए, किसके साथ सोता हूँ।</t>
   </si>
   <si>
     <t>सुनो, यार, हम दोनों में से,</t>
   </si>
   <si>
-    <t>शर्त लगाता हूँ मैं ही हूँ जो हाल में किसी शादीशुदा औरत के साथ सोया।</t>
+    <t>शर्त लगाता हूँ मैं ही हूँ जो हाल में  किसी शादीशुदा औरत के साथ सोया।</t>
   </si>
   <si>
     <t>चार्ली, एलन बोल रहा हूँ। तुम्हारा भाई।</t>
@@ -2149,22 +2152,22 @@
     <t>यह कुछ ऐसा नहीं जिस पर डींगें मारी जाएँ?</t>
   </si>
   <si>
-    <t>तुम्हें अंदाज़ा भी है कि यह कितना दर्दनाक है</t>
-  </si>
-  <si>
-    <t>जब अपने खुद के बेटे के तलाक के बारे में सड़क पर सुना हो?</t>
+    <t>तुम्हें अंदाज़ा भी है  कि यह कितना दर्दनाक है</t>
+  </si>
+  <si>
+    <t>जब अपने खुद के बेटे के  तलाक के बारे में सड़क पर सुना हो?</t>
   </si>
   <si>
     <t>क्या तलाक? कौन सी सड़क?</t>
   </si>
   <si>
-    <t>कोई ख़ास बात नहीं, बस बात करना चाहता था।</t>
+    <t>कोई ख़ास बात नहीं,  बस बात करना चाहता था।</t>
   </si>
   <si>
     <t>आप मेरे घर में कैसे आई?</t>
   </si>
   <si>
-    <t>मैं तुम्हारे भाई के मुश्किल समय में मदद के लिए आई।</t>
+    <t>मैं तुम्हारे भाई के  मुश्किल समय में मदद के लिए आई।</t>
   </si>
   <si>
     <t>मेरे साथ यह कैसे कर सकते हो?</t>
@@ -2179,13 +2182,13 @@
     <t>तो मुझे जूडिथ से अपॉइंटमेंट लेनी होगी,</t>
   </si>
   <si>
-    <t>हमें पता है, वह मुझसे कभी खुश नहीं रही।</t>
-  </si>
-  <si>
-    <t>क्या होगा अगर वहाँ कोई दूसरा आदमी हो? उसी घर में अविवाहित?</t>
-  </si>
-  <si>
-    <t>मेरी पत्नी ने मुझे निकाल दिया, और मेरी जीने की इच्छा ख़त्म हो रही है।</t>
+    <t>हमें पता है,  वह मुझसे कभी खुश नहीं रही।</t>
+  </si>
+  <si>
+    <t>क्या होगा अगर वहाँ कोई दूसरा आदमी हो?  उसी घर में अविवाहित?</t>
+  </si>
+  <si>
+    <t>मेरी पत्नी ने मुझे निकाल दिया,  और मेरी जीने की इच्छा ख़त्म हो रही है।</t>
   </si>
   <si>
     <t>क्या हमने उस बारे में भी सोचा है?</t>
@@ -2194,7 +2197,7 @@
     <t>मुझे लगता है कि वह अब सोच रहा है, माँ।</t>
   </si>
   <si>
-    <t>आइस्ड टी, दादी माँ। नन्हे फ़रिश्ते।</t>
+    <t>-आपकी आइस्ड टी, दादी माँ।  -शुक्रिया, नन्हे फ़रिश्ते।</t>
   </si>
   <si>
     <t>जानू, नीबू की फाॉँक माँगी थी।</t>
@@ -2206,10 +2209,10 @@
     <t>तुम और जेक मेरे साथ रहने आओगे।</t>
   </si>
   <si>
-    <t>आखिरकार, इतने बड़े घर में मैं अकेले रहती हूँ।</t>
-  </si>
-  <si>
-    <t>यह बहुत विचारशील है, पर जूडिथ और मैं जल्दी ही सब सुलझा लेंगे,</t>
+    <t>आखिरकार, इतने बड़े घर में  मैं अकेले रहती हूँ।</t>
+  </si>
+  <si>
+    <t>यह बहुत विचारशील है, पर जूडिथ  और मैं जल्दी ही सब सुलझा लेंगे,</t>
   </si>
   <si>
     <t>मैं अपने घर वापस चला जाऊँगा।</t>
@@ -2221,52 +2224,52 @@
     <t>जो कहा उसके बारे में सोचो।</t>
   </si>
   <si>
-    <t>तुम मेरे बेटे हो, और मेरे घर में और मेरे दिल में हमेशा</t>
+    <t>तुम मेरे बेटे हो,  और मेरे घर में और मेरे दिल में हमेशा</t>
   </si>
   <si>
     <t>तुम्हारे लिए जगह रहेगी।</t>
   </si>
   <si>
-    <t>जब भी मौका मिले, मुझे वाकई अच्छा लगेगा, मुझे नहीं पता</t>
-  </si>
-  <si>
-    <t>लव यू टू, माँ। कम। बहुत देर से।</t>
-  </si>
-  <si>
-    <t>वेगास अच्छा था? था।</t>
+    <t>जब भी मौका मिले,  मुझे वाकई अच्छा लगेगा, मुझे नहीं पता</t>
+  </si>
+  <si>
+    <t>-आई लव यू टू, माँ।  -बहुत कम। बहुत देर से।</t>
+  </si>
+  <si>
+    <t>-तो, वेगास अच्छा था?  -ठीक था।</t>
   </si>
   <si>
     <t>एलन, इस बारे में जानकर दुख हुआ।</t>
   </si>
   <si>
-    <t>मुझे वाकई तुम्हें इस स्थिति में डालने के लिए खेद है।</t>
-  </si>
-  <si>
-    <t>अपने दुख के लिए तुमको दोष देना मेरी गलती थी।</t>
-  </si>
-  <si>
-    <t>ज़रूरी बात यह है कि हम यहाँ हैं और अपनी शादी बचाने की कोशिश कर रहे हैं।</t>
-  </si>
-  <si>
-    <t>उस ऑक्सीजन की वजह से होगी जो वे कसीनो में डालते हैं।</t>
-  </si>
-  <si>
-    <t>मैंने देखा कि अलग होना हम दोनों के लिए बहुत अच्छा रहा।</t>
+    <t>मुझे वाकई तुम्हें  इस स्थिति में डालने के लिए खेद है।</t>
+  </si>
+  <si>
+    <t>अपने दुख के लिए  तुमको दोष देना मेरी गलती थी।</t>
+  </si>
+  <si>
+    <t>ज़रूरी बात यह है कि हम यहाँ हैं  और अपनी शादी बचाने की कोशिश कर रहे हैं।</t>
+  </si>
+  <si>
+    <t>उस ऑक्सीजन की वजह से होगी  जो वे कसीनो में डालते हैं।</t>
+  </si>
+  <si>
+    <t>मैंने देखा कि अलग होना  हम दोनों के लिए बहुत अच्छा रहा।</t>
   </si>
   <si>
     <t>तो, तुम कहाँ जाओगे, होटल में? वाह।</t>
   </si>
   <si>
-    <t>मैं वह परेशान करने वाला आदमी नहीं रहा जिसे तुमने</t>
+    <t>मैं वह परेशान करने वाला  आदमी नहीं रहा जिसे तुमने</t>
   </si>
   <si>
     <t>साढ़े चार दिन पहले घर से निकाला।</t>
   </si>
   <si>
-    <t>बढ़िया है।</t>
-  </si>
-  <si>
-    <t>तुम चिंतित थी कि मेरे भाई के साथ कैसे रहेगा,</t>
+    <t>-एलन।  -जेक बढ़िया है।</t>
+  </si>
+  <si>
+    <t>तुम चिंतित थी  कि मेरे भाई के साथ कैसे रहेगा,</t>
   </si>
   <si>
     <t>पर चार्ली की बच्चों से खूब पटती है।</t>
@@ -2278,10 +2281,10 @@
     <t>मैं भी।</t>
   </si>
   <si>
-    <t>में एक डॉलर डालता हूँ और पाँच डॉलर की चाल चलता हूँ।</t>
-  </si>
-  <si>
-    <t>देखना चाहूँगा। भी।</t>
+    <t>में एक डॉलर डालता हूँ  और पाँच डॉलर की चाल चलता हूँ।</t>
+  </si>
+  <si>
+    <t>-कार्ड देखना चाहूँगा।  -मैं भी।</t>
   </si>
   <si>
     <t>रानियाँ पूरी नौ।</t>
@@ -2293,7 +2296,7 @@
     <t>मुझे यह बच्चा पसंद है।</t>
   </si>
   <si>
-    <t>मेरे ख़याल से हमें इसे हमारी शादी के लिए नई शुरुआत की तरह देखना चाहिए।</t>
+    <t>मेरे ख़याल से हमें इसे हमारी शादी के लिए  नई शुरुआत की तरह देखना चाहिए।</t>
   </si>
   <si>
     <t>पुनर्जन्म। एक पुनर्जागरण, अगर तुम चाहो।</t>
@@ -2311,13 +2314,13 @@
     <t>मैं तुम्हें देखूँगा</t>
   </si>
   <si>
-    <t>ख़ैर, हाँ, मुझे लगता है कि तुम यहाँ रह सकते हो।</t>
-  </si>
-  <si>
-    <t>और डॉलर की चाल चलूगा।</t>
-  </si>
-  <si>
-    <t>लगता है उसने फँसा लिया। झाँसा दे रहा है।</t>
+    <t>ख़ैर, हाँ, मुझे लगता है  कि तुम यहाँ रह सकते हो।</t>
+  </si>
+  <si>
+    <t>और 20 डॉलर की चाल चलूगा।</t>
+  </si>
+  <si>
+    <t>-मुझे लगता है उसने फँसा लिया।  -वह झाँसा दे रहा है।</t>
   </si>
   <si>
     <t>जब झाँसा देता है तो कान खींचता है।</t>
@@ -2329,7 +2332,7 @@
     <t>धत्‌, यहाँ क्या चल रहा है?</t>
   </si>
   <si>
-    <t>आपने कहा।</t>
+    <t>आपने "धत्‌" कहा।</t>
   </si>
   <si>
     <t>एक डॉलर जार में डालो।</t>
@@ -2341,7 +2344,7 @@
     <t>चार्ली, तुमसे अकेले में बात कर सकता हूँ?</t>
   </si>
   <si>
-    <t>बाँटेगा? सोने जाओ!</t>
+    <t>-कौन बाँटेगा?  -जेक, सोने जाओ!</t>
   </si>
   <si>
     <t>ठीक है। जब तुम यहाँ आओगे तब मिलता हूँ।</t>
@@ -2353,7 +2356,7 @@
     <t>शायद नहीं। डिनर कैसा था?</t>
   </si>
   <si>
-    <t>तुमने बड़ों के साथ जेक को पोकर क्यों खिलाया?</t>
+    <t>तुमने बड़ों के साथ  जेक को पोकर क्यों खिलाया?</t>
   </si>
   <si>
     <t>बेशक मेरा भरोसा नहीं किया जा सकता।</t>
@@ -2362,16 +2365,16 @@
     <t>तो, डिनर कैसा था?</t>
   </si>
   <si>
-    <t>कुछ घंटों के लिए तुम्हें उसके साथ अकेले छोड़ता हूँ--</t>
-  </si>
-  <si>
-    <t>डिनर बढ़िया था। हमने वील पिकाटा खाई और वह समलैंगिक है!</t>
+    <t>कुछ घंटों के लिए  तुम्हें उसके साथ अकेले छोड़ता हूँ--</t>
+  </si>
+  <si>
+    <t>डिनर बढ़िया था। हमने  वील पिकाटा खाई और वह समलैंगिक है!</t>
   </si>
   <si>
     <t>जल्दी-जल्दी कर लेते हैं।</t>
   </si>
   <si>
-    <t>यह तुम्हारे लिए है, है</t>
+    <t>यह तुम्हारे लिए है, है न?</t>
   </si>
 </sst>
 </file>
@@ -2749,15 +2752,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C516"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:XFD79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -2787,7 +2790,7 @@
         <v>275</v>
       </c>
       <c r="C3" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -2806,7 +2809,7 @@
         <v>516</v>
       </c>
       <c r="C5" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2983,7 +2986,7 @@
         <v>285</v>
       </c>
       <c r="C23" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2994,7 +2997,7 @@
         <v>294</v>
       </c>
       <c r="C24" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -3005,7 +3008,7 @@
         <v>304</v>
       </c>
       <c r="C25" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -3016,7 +3019,7 @@
         <v>318</v>
       </c>
       <c r="C26" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -3051,7 +3054,7 @@
         <v>361</v>
       </c>
       <c r="C30" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -3070,7 +3073,7 @@
         <v>384</v>
       </c>
       <c r="C32" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -3081,7 +3084,7 @@
         <v>394</v>
       </c>
       <c r="C33" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -3092,7 +3095,7 @@
         <v>404</v>
       </c>
       <c r="C34" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -3103,7 +3106,7 @@
         <v>413</v>
       </c>
       <c r="C35" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -3114,7 +3117,7 @@
         <v>428</v>
       </c>
       <c r="C36" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -3125,7 +3128,7 @@
         <v>438</v>
       </c>
       <c r="C37" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -3136,7 +3139,7 @@
         <v>448</v>
       </c>
       <c r="C38" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -3163,7 +3166,7 @@
         <v>481</v>
       </c>
       <c r="C41" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -3182,7 +3185,7 @@
         <v>505</v>
       </c>
       <c r="C43" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -3193,7 +3196,7 @@
         <v>515</v>
       </c>
       <c r="C44" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -4780,6 +4783,9 @@
       <c r="B208" t="s">
         <v>265</v>
       </c>
+      <c r="C208" t="s">
+        <v>648</v>
+      </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A209">
@@ -4797,7 +4803,7 @@
         <v>267</v>
       </c>
       <c r="C210" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.35">
@@ -4808,7 +4814,7 @@
         <v>268</v>
       </c>
       <c r="C211" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.35">
@@ -4819,7 +4825,7 @@
         <v>269</v>
       </c>
       <c r="C212" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.35">
@@ -4838,7 +4844,7 @@
         <v>272</v>
       </c>
       <c r="C214" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.35">
@@ -4857,7 +4863,7 @@
         <v>274</v>
       </c>
       <c r="C216" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.35">
@@ -4876,7 +4882,7 @@
         <v>277</v>
       </c>
       <c r="C218" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.35">
@@ -4895,7 +4901,7 @@
         <v>279</v>
       </c>
       <c r="C220" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.35">
@@ -4906,7 +4912,7 @@
         <v>280</v>
       </c>
       <c r="C221" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.35">
@@ -4925,7 +4931,7 @@
         <v>282</v>
       </c>
       <c r="C223" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.35">
@@ -4944,7 +4950,7 @@
         <v>284</v>
       </c>
       <c r="C225" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.35">
@@ -4963,7 +4969,7 @@
         <v>287</v>
       </c>
       <c r="C227" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.35">
@@ -4990,7 +4996,7 @@
         <v>290</v>
       </c>
       <c r="C230" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.35">
@@ -5001,7 +5007,7 @@
         <v>291</v>
       </c>
       <c r="C231" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.35">
@@ -5012,7 +5018,7 @@
         <v>292</v>
       </c>
       <c r="C232" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.35">
@@ -5023,7 +5029,7 @@
         <v>293</v>
       </c>
       <c r="C233" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.35">
@@ -5034,7 +5040,7 @@
         <v>295</v>
       </c>
       <c r="C234" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.35">
@@ -5045,7 +5051,7 @@
         <v>296</v>
       </c>
       <c r="C235" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.35">
@@ -5064,7 +5070,7 @@
         <v>298</v>
       </c>
       <c r="C237" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.35">
@@ -5075,7 +5081,7 @@
         <v>299</v>
       </c>
       <c r="C238" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.35">
@@ -5086,7 +5092,7 @@
         <v>300</v>
       </c>
       <c r="C239" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.35">
@@ -5105,7 +5111,7 @@
         <v>302</v>
       </c>
       <c r="C241" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.35">
@@ -5132,7 +5138,7 @@
         <v>306</v>
       </c>
       <c r="C244" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.35">
@@ -5183,7 +5189,7 @@
         <v>312</v>
       </c>
       <c r="C250" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.35">
@@ -5194,7 +5200,7 @@
         <v>313</v>
       </c>
       <c r="C251" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.35">
@@ -5205,7 +5211,7 @@
         <v>314</v>
       </c>
       <c r="C252" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.35">
@@ -5224,7 +5230,7 @@
         <v>316</v>
       </c>
       <c r="C254" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.35">
@@ -5235,7 +5241,7 @@
         <v>317</v>
       </c>
       <c r="C255" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.35">
@@ -5254,7 +5260,7 @@
         <v>320</v>
       </c>
       <c r="C257" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.35">
@@ -5281,7 +5287,7 @@
         <v>323</v>
       </c>
       <c r="C260" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.35">
@@ -5292,7 +5298,7 @@
         <v>324</v>
       </c>
       <c r="C261" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.35">
@@ -5303,7 +5309,7 @@
         <v>325</v>
       </c>
       <c r="C262" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.35">
@@ -5314,7 +5320,7 @@
         <v>326</v>
       </c>
       <c r="C263" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.35">
@@ -5341,7 +5347,7 @@
         <v>330</v>
       </c>
       <c r="C266" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.35">
@@ -5352,7 +5358,7 @@
         <v>331</v>
       </c>
       <c r="C267" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.35">
@@ -5363,7 +5369,7 @@
         <v>332</v>
       </c>
       <c r="C268" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.35">
@@ -5430,7 +5436,7 @@
         <v>341</v>
       </c>
       <c r="C276" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.35">
@@ -5441,7 +5447,7 @@
         <v>342</v>
       </c>
       <c r="C277" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.35">
@@ -5476,7 +5482,7 @@
         <v>346</v>
       </c>
       <c r="C281" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.35">
@@ -5487,7 +5493,7 @@
         <v>347</v>
       </c>
       <c r="C282" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.35">
@@ -5530,7 +5536,7 @@
         <v>353</v>
       </c>
       <c r="C287" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.35">
@@ -5541,7 +5547,7 @@
         <v>354</v>
       </c>
       <c r="C288" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.35">
@@ -5560,7 +5566,7 @@
         <v>356</v>
       </c>
       <c r="C290" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.35">
@@ -5571,7 +5577,7 @@
         <v>357</v>
       </c>
       <c r="C291" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.35">
@@ -5590,7 +5596,7 @@
         <v>359</v>
       </c>
       <c r="C293" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.35">
@@ -5609,7 +5615,7 @@
         <v>362</v>
       </c>
       <c r="C295" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.35">
@@ -5644,7 +5650,7 @@
         <v>366</v>
       </c>
       <c r="C299" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.35">
@@ -5655,7 +5661,7 @@
         <v>367</v>
       </c>
       <c r="C300" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.35">
@@ -5666,7 +5672,7 @@
         <v>368</v>
       </c>
       <c r="C301" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.35">
@@ -5685,7 +5691,7 @@
         <v>371</v>
       </c>
       <c r="C303" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.35">
@@ -5696,7 +5702,7 @@
         <v>372</v>
       </c>
       <c r="C304" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.35">
@@ -5707,7 +5713,7 @@
         <v>373</v>
       </c>
       <c r="C305" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.35">
@@ -5718,7 +5724,7 @@
         <v>374</v>
       </c>
       <c r="C306" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.35">
@@ -5729,7 +5735,7 @@
         <v>375</v>
       </c>
       <c r="C307" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.35">
@@ -5748,7 +5754,7 @@
         <v>377</v>
       </c>
       <c r="C309" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.35">
@@ -5759,7 +5765,7 @@
         <v>378</v>
       </c>
       <c r="C310" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.35">
@@ -5770,7 +5776,7 @@
         <v>379</v>
       </c>
       <c r="C311" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.35">
@@ -5781,7 +5787,7 @@
         <v>380</v>
       </c>
       <c r="C312" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.35">
@@ -5792,7 +5798,7 @@
         <v>381</v>
       </c>
       <c r="C313" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.35">
@@ -5803,7 +5809,7 @@
         <v>382</v>
       </c>
       <c r="C314" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.35">
@@ -5814,7 +5820,7 @@
         <v>383</v>
       </c>
       <c r="C315" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.35">
@@ -5825,7 +5831,7 @@
         <v>385</v>
       </c>
       <c r="C316" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.35">
@@ -5868,7 +5874,7 @@
         <v>390</v>
       </c>
       <c r="C321" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.35">
@@ -5879,7 +5885,7 @@
         <v>391</v>
       </c>
       <c r="C322" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.35">
@@ -5890,7 +5896,7 @@
         <v>392</v>
       </c>
       <c r="C323" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.35">
@@ -5909,7 +5915,7 @@
         <v>395</v>
       </c>
       <c r="C325" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.35">
@@ -5928,7 +5934,7 @@
         <v>397</v>
       </c>
       <c r="C327" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.35">
@@ -5939,7 +5945,7 @@
         <v>398</v>
       </c>
       <c r="C328" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.35">
@@ -5950,7 +5956,7 @@
         <v>399</v>
       </c>
       <c r="C329" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.35">
@@ -5961,7 +5967,7 @@
         <v>400</v>
       </c>
       <c r="C330" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.35">
@@ -5972,7 +5978,7 @@
         <v>401</v>
       </c>
       <c r="C331" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.35">
@@ -5983,7 +5989,7 @@
         <v>402</v>
       </c>
       <c r="C332" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.35">
@@ -5994,7 +6000,7 @@
         <v>403</v>
       </c>
       <c r="C333" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.35">
@@ -6005,7 +6011,7 @@
         <v>405</v>
       </c>
       <c r="C334" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.35">
@@ -6016,7 +6022,7 @@
         <v>406</v>
       </c>
       <c r="C335" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.35">
@@ -6043,7 +6049,7 @@
         <v>409</v>
       </c>
       <c r="C338" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.35">
@@ -6054,7 +6060,7 @@
         <v>410</v>
       </c>
       <c r="C339" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.35">
@@ -6065,7 +6071,7 @@
         <v>411</v>
       </c>
       <c r="C340" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.35">
@@ -6092,7 +6098,7 @@
         <v>415</v>
       </c>
       <c r="C343" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.35">
@@ -6103,7 +6109,7 @@
         <v>416</v>
       </c>
       <c r="C344" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.35">
@@ -6114,7 +6120,7 @@
         <v>417</v>
       </c>
       <c r="C345" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.35">
@@ -6125,7 +6131,7 @@
         <v>418</v>
       </c>
       <c r="C346" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.35">
@@ -6136,7 +6142,7 @@
         <v>420</v>
       </c>
       <c r="C347" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.35">
@@ -6147,7 +6153,7 @@
         <v>421</v>
       </c>
       <c r="C348" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.35">
@@ -6158,7 +6164,7 @@
         <v>422</v>
       </c>
       <c r="C349" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.35">
@@ -6177,7 +6183,7 @@
         <v>424</v>
       </c>
       <c r="C351" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.35">
@@ -6188,7 +6194,7 @@
         <v>425</v>
       </c>
       <c r="C352" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.35">
@@ -6199,7 +6205,7 @@
         <v>426</v>
       </c>
       <c r="C353" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.35">
@@ -6258,7 +6264,7 @@
         <v>434</v>
       </c>
       <c r="C360" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.35">
@@ -6285,7 +6291,7 @@
         <v>437</v>
       </c>
       <c r="C363" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.35">
@@ -6296,7 +6302,7 @@
         <v>439</v>
       </c>
       <c r="C364" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.35">
@@ -6307,7 +6313,7 @@
         <v>440</v>
       </c>
       <c r="C365" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.35">
@@ -6318,7 +6324,7 @@
         <v>441</v>
       </c>
       <c r="C366" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.35">
@@ -6329,7 +6335,7 @@
         <v>442</v>
       </c>
       <c r="C367" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.35">
@@ -6340,7 +6346,7 @@
         <v>443</v>
       </c>
       <c r="C368" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.35">
@@ -6351,7 +6357,7 @@
         <v>444</v>
       </c>
       <c r="C369" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.35">
@@ -6362,7 +6368,7 @@
         <v>445</v>
       </c>
       <c r="C370" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.35">
@@ -6373,7 +6379,7 @@
         <v>446</v>
       </c>
       <c r="C371" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.35">
@@ -6384,7 +6390,7 @@
         <v>447</v>
       </c>
       <c r="C372" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.35">
@@ -6395,7 +6401,7 @@
         <v>449</v>
       </c>
       <c r="C373" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.35">
@@ -6406,7 +6412,7 @@
         <v>450</v>
       </c>
       <c r="C374" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.35">
@@ -6417,7 +6423,7 @@
         <v>451</v>
       </c>
       <c r="C375" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.35">
@@ -6428,7 +6434,7 @@
         <v>452</v>
       </c>
       <c r="C376" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.35">
@@ -6439,7 +6445,7 @@
         <v>453</v>
       </c>
       <c r="C377" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.35">
@@ -6450,7 +6456,7 @@
         <v>454</v>
       </c>
       <c r="C378" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.35">
@@ -6477,7 +6483,7 @@
         <v>457</v>
       </c>
       <c r="C381" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.35">
@@ -6488,7 +6494,7 @@
         <v>458</v>
       </c>
       <c r="C382" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.35">
@@ -6515,7 +6521,7 @@
         <v>461</v>
       </c>
       <c r="C385" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.35">
@@ -6534,7 +6540,7 @@
         <v>464</v>
       </c>
       <c r="C387" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.35">
@@ -6553,7 +6559,7 @@
         <v>466</v>
       </c>
       <c r="C389" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.35">
@@ -6572,7 +6578,7 @@
         <v>468</v>
       </c>
       <c r="C391" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.35">
@@ -6591,7 +6597,7 @@
         <v>470</v>
       </c>
       <c r="C393" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.35">
@@ -6602,7 +6608,7 @@
         <v>471</v>
       </c>
       <c r="C394" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.35">
@@ -6613,7 +6619,7 @@
         <v>473</v>
       </c>
       <c r="C395" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.35">
@@ -6648,7 +6654,7 @@
         <v>477</v>
       </c>
       <c r="C399" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.35">
@@ -6667,7 +6673,7 @@
         <v>479</v>
       </c>
       <c r="C401" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.35">
@@ -6678,7 +6684,7 @@
         <v>480</v>
       </c>
       <c r="C402" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.35">
@@ -6689,7 +6695,7 @@
         <v>482</v>
       </c>
       <c r="C403" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.35">
@@ -6716,7 +6722,7 @@
         <v>485</v>
       </c>
       <c r="C406" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.35">
@@ -6727,7 +6733,7 @@
         <v>486</v>
       </c>
       <c r="C407" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.35">
@@ -6746,7 +6752,7 @@
         <v>488</v>
       </c>
       <c r="C409" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.35">
@@ -6805,7 +6811,7 @@
         <v>495</v>
       </c>
       <c r="C416" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.35">
@@ -6816,7 +6822,7 @@
         <v>497</v>
       </c>
       <c r="C417" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.35">
@@ -6827,7 +6833,7 @@
         <v>498</v>
       </c>
       <c r="C418" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.35">
@@ -6838,7 +6844,7 @@
         <v>499</v>
       </c>
       <c r="C419" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.35">
@@ -6857,7 +6863,7 @@
         <v>501</v>
       </c>
       <c r="C421" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.35">
@@ -6876,7 +6882,7 @@
         <v>503</v>
       </c>
       <c r="C423" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.35">
@@ -6895,7 +6901,7 @@
         <v>506</v>
       </c>
       <c r="C425" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.35">
@@ -6906,7 +6912,7 @@
         <v>507</v>
       </c>
       <c r="C426" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.35">
@@ -6917,7 +6923,7 @@
         <v>508</v>
       </c>
       <c r="C427" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.35">
@@ -6928,7 +6934,7 @@
         <v>509</v>
       </c>
       <c r="C428" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.35">
@@ -6947,7 +6953,7 @@
         <v>511</v>
       </c>
       <c r="C430" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.35">
@@ -6958,7 +6964,7 @@
         <v>512</v>
       </c>
       <c r="C431" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.35">
@@ -6969,7 +6975,7 @@
         <v>513</v>
       </c>
       <c r="C432" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.35">
@@ -6980,7 +6986,7 @@
         <v>514</v>
       </c>
       <c r="C433" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>